<commit_message>
Permisos de la base de datos
</commit_message>
<xml_diff>
--- a/Actividades/Femp03011/Flujo de fondos v1.xlsx
+++ b/Actividades/Femp03011/Flujo de fondos v1.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Femp03011\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED220E8-84A6-4B2C-9ED6-E689EB4B0B72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B47BBD03-94DA-414B-B33A-289FA1FC0061}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,9 +501,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Electrisidad </t>
-  </si>
-  <si>
     <t>Dolares</t>
   </si>
   <si>
@@ -529,12 +520,15 @@
   </si>
   <si>
     <t xml:space="preserve">Sin proyecto </t>
+  </si>
+  <si>
+    <t>Electricidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$UYU]_-;\-* #,##0.00\ [$UYU]_-;_-* &quot;-&quot;??\ [$UYU]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$USD]_-;\-* #,##0.00\ [$USD]_-;_-* &quot;-&quot;??\ [$USD]_-;_-@_-"/>
@@ -1193,31 +1187,49 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1247,44 +1259,26 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1328,7 +1322,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E0A728E-BC35-4AA8-84D0-D45961123560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8E0A728E-BC35-4AA8-84D0-D45961123560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1406,7 +1400,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1458,7 +1452,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1652,18 +1646,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A1C63E0-E69E-4EA5-B6E3-0D1DCF0538CA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,20 +1675,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="79"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="85"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -1714,19 +1708,19 @@
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="86" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="81"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="87"/>
     </row>
     <row r="4" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -1746,12 +1740,12 @@
       <c r="A5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="88">
         <f>(B9-B10-B11-B12)*(1-B14)+B11-B16-B13</f>
         <v>1371393.9246666685</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1776,13 +1770,13 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
+      <c r="A7" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1793,14 +1787,14 @@
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="86" t="s">
+      <c r="B8" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="86"/>
+      <c r="E8" s="72"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1813,15 +1807,15 @@
       <c r="A9" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="83">
+      <c r="B9" s="89">
         <f>SUM(B25:E25)</f>
         <v>12994638.064000001</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="95">
+      <c r="C9" s="89"/>
+      <c r="D9" s="74">
         <v>0</v>
       </c>
-      <c r="E9" s="95"/>
+      <c r="E9" s="74"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1834,15 +1828,15 @@
       <c r="A10" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="84">
+      <c r="B10" s="76">
         <f>SUM(B45:C45)</f>
         <v>10456506.719999999</v>
       </c>
-      <c r="C10" s="84"/>
-      <c r="D10" s="96">
+      <c r="C10" s="76"/>
+      <c r="D10" s="75">
         <v>0</v>
       </c>
-      <c r="E10" s="96"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1855,15 +1849,15 @@
       <c r="A11" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="84">
+      <c r="B11" s="76">
         <f>SUM(E49:E77)</f>
         <v>3501.6666666666665</v>
       </c>
-      <c r="C11" s="84"/>
-      <c r="D11" s="96">
+      <c r="C11" s="76"/>
+      <c r="D11" s="75">
         <v>0</v>
       </c>
-      <c r="E11" s="96"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1876,12 +1870,12 @@
       <c r="A12" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="77">
         <v>0</v>
       </c>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="70"/>
+      <c r="C12" s="79"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="78"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1894,12 +1888,12 @@
       <c r="A13" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="74">
+      <c r="B13" s="80">
         <v>0</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="76"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="82"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1912,12 +1906,12 @@
       <c r="A14" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="66">
+      <c r="B14" s="92">
         <v>0.25</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
+      <c r="E14" s="94"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1927,17 +1921,17 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="69" t="s">
+      <c r="B15" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="69" t="s">
+      <c r="C15" s="78"/>
+      <c r="D15" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="70"/>
+      <c r="E15" s="78"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1947,16 +1941,16 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
-      <c r="B16" s="71">
+      <c r="A16" s="71"/>
+      <c r="B16" s="95">
         <f>D16*H48</f>
         <v>533080</v>
       </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="64">
+      <c r="C16" s="96"/>
+      <c r="D16" s="90">
         <v>13327</v>
       </c>
-      <c r="E16" s="65"/>
+      <c r="E16" s="91"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -1969,12 +1963,12 @@
       <c r="A17" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="69" t="s">
+      <c r="B17" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="70"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="78"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -2014,7 +2008,7 @@
         <v>17</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -2178,15 +2172,15 @@
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="91" t="s">
+      <c r="B27" s="65"/>
+      <c r="C27" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="91"/>
-      <c r="E27" s="92"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -2448,7 +2442,7 @@
         <v>26</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -2504,10 +2498,10 @@
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="88" t="s">
+      <c r="G40" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="H40" s="88"/>
+      <c r="H40" s="70"/>
       <c r="I40" s="1" t="s">
         <v>46</v>
       </c>
@@ -2535,11 +2529,11 @@
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
-      <c r="G41" s="88" t="s">
+      <c r="G41" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="H41" s="88"/>
-      <c r="I41" s="32">
+      <c r="H41" s="70"/>
+      <c r="I41" s="37">
         <v>657</v>
       </c>
       <c r="J41" s="1">
@@ -2566,11 +2560,11 @@
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
-      <c r="G42" s="88" t="s">
+      <c r="G42" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="88"/>
-      <c r="I42" s="32">
+      <c r="H42" s="70"/>
+      <c r="I42" s="37">
         <v>30</v>
       </c>
       <c r="J42" s="1">
@@ -2597,11 +2591,11 @@
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
-      <c r="G43" s="88" t="s">
+      <c r="G43" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="H43" s="88"/>
-      <c r="I43" s="32">
+      <c r="H43" s="70"/>
+      <c r="I43" s="37">
         <v>150</v>
       </c>
       <c r="J43" s="1">
@@ -2617,11 +2611,11 @@
       <c r="D44" s="48"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
-      <c r="G44" s="88" t="s">
+      <c r="G44" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="H44" s="88"/>
-      <c r="I44" s="32">
+      <c r="H44" s="70"/>
+      <c r="I44" s="37">
         <f>SUM(I41:I43)</f>
         <v>837</v>
       </c>
@@ -2671,21 +2665,21 @@
       <c r="L46" s="11"/>
     </row>
     <row r="47" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A47" s="89" t="s">
+      <c r="A47" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="91" t="s">
+      <c r="B47" s="69"/>
+      <c r="C47" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="D47" s="91"/>
-      <c r="E47" s="92"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="67"/>
       <c r="F47" s="10"/>
       <c r="G47" s="1" t="s">
         <v>48</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
@@ -2931,7 +2925,7 @@
         <v>16</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
@@ -3127,7 +3121,7 @@
         <v>30</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
@@ -3150,7 +3144,7 @@
         <v>150</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -3167,13 +3161,13 @@
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="H68" s="1">
         <v>88</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
@@ -3392,15 +3386,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="D8:E8"/>
@@ -3412,16 +3403,19 @@
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modificacion en fecharegistro en lugar y algo mas de persistencia
</commit_message>
<xml_diff>
--- a/Actividades/Femp03011/Flujo de fondos v1.xlsx
+++ b/Actividades/Femp03011/Flujo de fondos v1.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Femp03011\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FBD9D6-BE55-42C8-8D16-9EAA55CB2462}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t xml:space="preserve">Formula: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Valor: </t>
   </si>
   <si>
     <r>
@@ -330,9 +333,6 @@
   </si>
   <si>
     <t>Soporte (todo el mes) Año 4</t>
-  </si>
-  <si>
-    <t>Fonaza, BPS, BSE?</t>
   </si>
   <si>
     <t xml:space="preserve">Prestamo </t>
@@ -524,11 +524,20 @@
   <si>
     <t>Electricidad</t>
   </si>
+  <si>
+    <t>Inflacion:</t>
+  </si>
+  <si>
+    <t>(Igual para los sueldos)</t>
+  </si>
+  <si>
+    <t>Flujo de fondos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$UYU]_-;\-* #,##0.00\ [$UYU]_-;_-* &quot;-&quot;??\ [$UYU]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$USD]_-;\-* #,##0.00\ [$USD]_-;_-* &quot;-&quot;??\ [$USD]_-;_-@_-"/>
@@ -1149,7 +1158,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1187,6 +1195,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,38 +1215,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1259,26 +1271,23 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1322,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8E0A728E-BC35-4AA8-84D0-D45961123560}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E0A728E-BC35-4AA8-84D0-D45961123560}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1400,7 +1409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1452,7 +1461,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1646,24 +1655,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I68" sqref="I68"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
@@ -1671,24 +1680,24 @@
     <col min="7" max="7" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="99.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85"/>
+      <c r="A1" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -1708,19 +1717,19 @@
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="86" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="87"/>
+      <c r="B3" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="87"/>
+      <c r="L3" s="88"/>
     </row>
     <row r="4" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A4" s="13"/>
@@ -1738,14 +1747,14 @@
     </row>
     <row r="5" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="88">
+        <v>83</v>
+      </c>
+      <c r="B5" s="89">
         <f>(B9-B10-B11-B12)*(1-B14)+B11-B16-B13</f>
-        <v>1371393.9246666685</v>
-      </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
+        <v>1453140.6635241194</v>
+      </c>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1770,13 +1779,13 @@
       <c r="L6" s="11"/>
     </row>
     <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
+      <c r="A7" s="94" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1787,14 +1796,14 @@
     </row>
     <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72" t="s">
-        <v>81</v>
-      </c>
-      <c r="E8" s="72"/>
+      <c r="B8" s="93" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="93"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1804,18 +1813,18 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="89">
+      <c r="A9" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="90">
         <f>SUM(B25:E25)</f>
-        <v>12994638.064000001</v>
-      </c>
-      <c r="C9" s="89"/>
-      <c r="D9" s="74">
+        <v>13648611.974859614</v>
+      </c>
+      <c r="C9" s="90"/>
+      <c r="D9" s="95">
         <v>0</v>
       </c>
-      <c r="E9" s="74"/>
+      <c r="E9" s="95"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1825,18 +1834,18 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="63" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="76">
+      <c r="A10" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="91">
         <f>SUM(B45:C45)</f>
-        <v>10456506.719999999</v>
-      </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="75">
+        <v>11001484.979049677</v>
+      </c>
+      <c r="C10" s="91"/>
+      <c r="D10" s="96">
         <v>0</v>
       </c>
-      <c r="E10" s="75"/>
+      <c r="E10" s="96"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -1846,18 +1855,18 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A11" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="76">
+      <c r="A11" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="91">
         <f>SUM(E49:E77)</f>
         <v>3501.6666666666665</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="75">
+      <c r="C11" s="91"/>
+      <c r="D11" s="96">
         <v>0</v>
       </c>
-      <c r="E11" s="75"/>
+      <c r="E11" s="96"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1867,15 +1876,15 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="77">
+      <c r="A12" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="79">
         <v>0</v>
       </c>
-      <c r="C12" s="79"/>
-      <c r="D12" s="79"/>
-      <c r="E12" s="78"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="80"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1885,15 +1894,15 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="63" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="80">
+      <c r="A13" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="71">
         <v>0</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="82"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
@@ -1903,15 +1912,15 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="92">
+      <c r="A14" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="76">
         <v>0.25</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="94"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="78"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
@@ -1921,17 +1930,17 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="78"/>
+      <c r="A15" s="92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="80"/>
+      <c r="D15" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="80"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
@@ -1941,16 +1950,16 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="95">
+      <c r="A16" s="92"/>
+      <c r="B16" s="81">
         <f>D16*H48</f>
         <v>533080</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="90">
+      <c r="C16" s="82"/>
+      <c r="D16" s="74">
         <v>13327</v>
       </c>
-      <c r="E16" s="91"/>
+      <c r="E16" s="75"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
@@ -1960,15 +1969,15 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="78"/>
+      <c r="A17" s="62" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="83"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="80"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
@@ -1992,23 +2001,23 @@
       <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="D19" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="E19" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="40" t="s">
-        <v>77</v>
+      <c r="F19" s="39" t="s">
+        <v>75</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
@@ -2019,7 +2028,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -2031,7 +2040,7 @@
       <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="40">
         <f>B20*E29+C20*E30+D20*E35+E36*E20</f>
         <v>6391294</v>
       </c>
@@ -2044,7 +2053,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1">
@@ -2052,9 +2061,9 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="41">
+      <c r="F21" s="40">
         <f>B21*E29+C21*E31+D21*E35+E36*E21</f>
-        <v>1330249.344</v>
+        <v>1436669.2915200002</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -2065,7 +2074,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
@@ -2073,9 +2082,9 @@
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="41">
+      <c r="F22" s="40">
         <f>B22*E29+C22*E32+D22*E35+E36*E22</f>
-        <v>1572792.3839999998</v>
+        <v>1713950.8927488001</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
@@ -2086,7 +2095,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
@@ -2094,9 +2103,9 @@
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="41">
+      <c r="F23" s="40">
         <f>B23*E29+C23*E33+D23*E35+E36*E23</f>
-        <v>1704202.7519999999</v>
+        <v>1877903.5215790081</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
@@ -2107,7 +2116,7 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="1">
@@ -2115,9 +2124,9 @@
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="42">
+      <c r="F24" s="41">
         <f>B24*E29+C24*E34+D24*E35+E36*E24</f>
-        <v>1996099.5840000003</v>
+        <v>2228794.2690118048</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
@@ -2127,28 +2136,28 @@
       <c r="L24" s="11"/>
     </row>
     <row r="25" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="44">
+      <c r="A25" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" s="43">
         <f>SUM(B20:B24)*E29</f>
         <v>460350</v>
       </c>
-      <c r="C25" s="44">
+      <c r="C25" s="43">
         <f>C20*E30+C21*E31+C22*E32+C23*E33+C24*E34</f>
-        <v>7635936.0640000012</v>
-      </c>
-      <c r="D25" s="44">
+        <v>8289909.974859613</v>
+      </c>
+      <c r="D25" s="43">
         <f>SUM(D20:D24)*E35</f>
         <v>0</v>
       </c>
-      <c r="E25" s="44">
+      <c r="E25" s="43">
         <f>SUM(E20:E24)*E36</f>
         <v>4898352</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="44">
         <f>SUM(F20:F24)</f>
-        <v>12994638.064000001</v>
+        <v>13648611.974859614</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
@@ -2173,11 +2182,11 @@
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="65"/>
       <c r="C27" s="66" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="66"/>
       <c r="E27" s="67"/>
@@ -2191,19 +2200,19 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="50" t="s">
         <v>22</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="51" t="s">
-        <v>23</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -2215,7 +2224,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="32">
         <f>(I41*(1+((J41/100)*0))+ I42*(1+((J42/100)*0)) + I43*(1+((J43/100)*0)))*H48*11</f>
@@ -2225,7 +2234,7 @@
       <c r="D29" s="5">
         <v>25</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="51">
         <f>SUM(B29:C29)*(1+(D29/100))</f>
         <v>460350</v>
       </c>
@@ -2239,7 +2248,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B30" s="32">
         <f>B39/12</f>
@@ -2252,7 +2261,7 @@
       <c r="D30" s="5">
         <v>20</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="51">
         <f>SUM(B30:C30)*(1+(D30/100))</f>
         <v>93871.999999999985</v>
       </c>
@@ -2266,22 +2275,22 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" s="32">
         <f>B40/12</f>
-        <v>40919.760000000002</v>
+        <v>44193.340800000005</v>
       </c>
       <c r="C31" s="32">
         <f t="shared" ref="B31:C34" si="0">C40/12</f>
-        <v>51458.666666666664</v>
+        <v>55575.360000000008</v>
       </c>
       <c r="D31" s="5">
         <v>20</v>
       </c>
-      <c r="E31" s="52">
+      <c r="E31" s="51">
         <f t="shared" ref="E31:E34" si="1">SUM(B31:C31)*(1+(D31/100))</f>
-        <v>110854.11199999999</v>
+        <v>119722.44096000002</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="34"/>
@@ -2293,22 +2302,22 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="32">
         <f t="shared" si="0"/>
-        <v>49932.359999999993</v>
+        <v>54991.887552000007</v>
       </c>
       <c r="C32" s="32">
         <f t="shared" si="0"/>
-        <v>59289.333333333336</v>
+        <v>64032.480000000003</v>
       </c>
       <c r="D32" s="5">
         <v>20</v>
       </c>
-      <c r="E32" s="52">
+      <c r="E32" s="51">
         <f t="shared" si="1"/>
-        <v>131066.03199999999</v>
+        <v>142829.24106240002</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="34"/>
@@ -2320,22 +2329,22 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="32">
         <f t="shared" si="0"/>
-        <v>55702.079999999994</v>
+        <v>62753.006776320013</v>
       </c>
       <c r="C33" s="32">
         <f t="shared" si="0"/>
-        <v>62645.333333333336</v>
+        <v>67656.960000000006</v>
       </c>
       <c r="D33" s="5">
         <v>20</v>
       </c>
-      <c r="E33" s="52">
+      <c r="E33" s="51">
         <f t="shared" si="1"/>
-        <v>142016.89599999998</v>
+        <v>156491.960131584</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="34"/>
@@ -2347,22 +2356,22 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="32">
         <f t="shared" si="0"/>
-        <v>67023.360000000001</v>
+        <v>77455.139792486429</v>
       </c>
       <c r="C34" s="32">
         <f t="shared" si="0"/>
-        <v>71594.666666666672</v>
+        <v>77322.240000000005</v>
       </c>
       <c r="D34" s="5">
         <v>20</v>
       </c>
-      <c r="E34" s="52">
+      <c r="E34" s="51">
         <f t="shared" si="1"/>
-        <v>166341.63200000001</v>
+        <v>185732.85575098373</v>
       </c>
       <c r="F34" s="10"/>
       <c r="G34" s="35"/>
@@ -2374,12 +2383,12 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="52">
+      <c r="E35" s="51">
         <f t="shared" ref="E35" si="2">SUM(B35:C35)*(1-(D35/100))</f>
         <v>0</v>
       </c>
@@ -2391,29 +2400,34 @@
       <c r="K35" s="10"/>
       <c r="L35" s="11"/>
     </row>
-    <row r="36" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="B36" s="54">
+    <row r="36" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="53">
         <f>I44*H48*2</f>
         <v>66960</v>
       </c>
-      <c r="C36" s="54">
+      <c r="C36" s="53">
         <v>4015000</v>
       </c>
-      <c r="D36" s="55">
+      <c r="D36" s="54">
         <v>20</v>
       </c>
-      <c r="E36" s="56">
+      <c r="E36" s="55">
         <f>SUM(B36:C36)*(1+(D36/100))</f>
         <v>4898352</v>
       </c>
       <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
+      <c r="H36" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" s="63">
+        <v>0.08</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="K36" s="10"/>
       <c r="L36" s="11"/>
     </row>
@@ -2432,17 +2446,17 @@
       <c r="L37" s="11"/>
     </row>
     <row r="38" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="C38" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>76</v>
+      <c r="D38" s="39" t="s">
+        <v>74</v>
       </c>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
@@ -2455,7 +2469,7 @@
     </row>
     <row r="39" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39" s="32">
         <f>(I41*(1+((J41/100)*0))+ I42*(1+((J42/100)*0)) + I43*(1+((J43/100)*0)))*H48*12</f>
@@ -2465,14 +2479,14 @@
         <f>H61+(H66*H48+H67*H48)*12+ C36</f>
         <v>4551960</v>
       </c>
-      <c r="D39" s="47">
+      <c r="D39" s="46">
         <f>SUM(B39:C39)</f>
         <v>4953720</v>
       </c>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H39" s="30"/>
       <c r="I39" s="27"/>
@@ -2482,58 +2496,58 @@
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" s="32">
-        <f>((I41*(1+((J41/100)*1)))+ (I42*(1+((J42/100)*1))) + (I43*(1+((J43/100)*1))))*H49*12</f>
-        <v>491037.12</v>
+        <f>((($I$41*(1+(($J$41/100)*1)))+ ($I$42*(1+(($J$42/100)*1))) + ($I$43*(1+(($J$43/100)*1))))*H49*12)*((1+$I$36)^1)</f>
+        <v>530320.08960000006</v>
       </c>
       <c r="C40" s="32">
-        <f>H62+(H66*H49+H67*H49)*12</f>
-        <v>617504</v>
-      </c>
-      <c r="D40" s="47">
+        <f>(H62+($H$66*H49+$H$67*H49)*12)*((1+$I$36)^1)</f>
+        <v>666904.32000000007</v>
+      </c>
+      <c r="D40" s="46">
         <f t="shared" ref="D40:D45" si="3">SUM(B40:C40)</f>
-        <v>1108541.1200000001</v>
+        <v>1197224.4096000001</v>
       </c>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H40" s="70"/>
       <c r="I40" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K40" s="10"/>
       <c r="L40" s="11"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="32">
-        <f>((I41*(1+((J41/100)*2)))+ (I42*(1+((J42/100)*2))) + (I43*(1+((J43/100)*2))))*H50*12</f>
-        <v>599188.31999999995</v>
+        <f>((($I$41*(1+(($J$41/100)*1)))+ ($I$42*(1+(($J$42/100)*1))) + ($I$43*(1+(($J$43/100)*1))))*H50*12)*((1+$I$36)^2)</f>
+        <v>659902.65062400012</v>
       </c>
       <c r="C41" s="32">
-        <f>H63+(H66*H50+H67*H50)*12</f>
-        <v>711472</v>
-      </c>
-      <c r="D41" s="47">
+        <f t="shared" ref="C41:C43" si="4">(H63+($H$66*H50+$H$67*H50)*12)*((1+$I$36)^1)</f>
+        <v>768389.76</v>
+      </c>
+      <c r="D41" s="46">
         <f t="shared" si="3"/>
-        <v>1310660.3199999998</v>
+        <v>1428292.4106240002</v>
       </c>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="70" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H41" s="70"/>
-      <c r="I41" s="37">
+      <c r="I41" s="36">
         <v>657</v>
       </c>
       <c r="J41" s="1">
@@ -2544,27 +2558,27 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="32">
-        <f>((I41*(1+((J41/100)*3)))+ (I42*(1+((J42/100)*3))) + (I43*(1+((J43/100)*3))))*H51*12</f>
-        <v>668424.95999999996</v>
+        <f>((($I$41*(1+(($J$41/100)*1)))+ ($I$42*(1+(($J$42/100)*1))) + ($I$43*(1+(($J$43/100)*1))))*H51*12)*((1+$I$36)^3)</f>
+        <v>753036.08131584013</v>
       </c>
       <c r="C42" s="32">
-        <f>H64+(H66*H51+H67*H51)*12</f>
-        <v>751744</v>
-      </c>
-      <c r="D42" s="47">
+        <f t="shared" si="4"/>
+        <v>811883.52000000002</v>
+      </c>
+      <c r="D42" s="46">
         <f t="shared" si="3"/>
-        <v>1420168.96</v>
+        <v>1564919.6013158401</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="70" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H42" s="70"/>
-      <c r="I42" s="37">
+      <c r="I42" s="36">
         <v>30</v>
       </c>
       <c r="J42" s="1">
@@ -2575,27 +2589,27 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="36">
-        <f>((I41*(1+((J41/100)*4)))+ (I42*(1+((J42/100)*4))) + (I43*(1+((J43/100)*4))))*H52*12</f>
-        <v>804280.32000000007</v>
+        <v>12</v>
+      </c>
+      <c r="B43" s="32">
+        <f>((($I$41*(1+(($J$41/100)*1)))+ ($I$42*(1+(($J$42/100)*1))) + ($I$43*(1+(($J$43/100)*1))))*H52*12)*((1+$I$36)^4)</f>
+        <v>929461.67750983709</v>
       </c>
       <c r="C43" s="32">
-        <f>H65+(H66*H52+H67*H52)*12</f>
-        <v>859136</v>
-      </c>
-      <c r="D43" s="47">
+        <f t="shared" si="4"/>
+        <v>927866.88</v>
+      </c>
+      <c r="D43" s="46">
         <f t="shared" si="3"/>
-        <v>1663416.3200000001</v>
+        <v>1857328.5575098372</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H43" s="70"/>
-      <c r="I43" s="37">
+      <c r="I43" s="36">
         <v>150</v>
       </c>
       <c r="J43" s="1">
@@ -2608,14 +2622,14 @@
       <c r="A44" s="16"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="48"/>
+      <c r="D44" s="47"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H44" s="70"/>
-      <c r="I44" s="37">
+      <c r="I44" s="36">
         <f>SUM(I41:I43)</f>
         <v>837</v>
       </c>
@@ -2624,20 +2638,20 @@
       <c r="L44" s="11"/>
     </row>
     <row r="45" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="B45" s="50">
+      <c r="A45" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="49">
         <f>SUM(B39:B43)</f>
-        <v>2964690.7199999997</v>
-      </c>
-      <c r="C45" s="50">
+        <v>3274480.4990496775</v>
+      </c>
+      <c r="C45" s="49">
         <f>SUM(C39:C44)</f>
-        <v>7491816</v>
-      </c>
-      <c r="D45" s="45">
+        <v>7727004.4799999995</v>
+      </c>
+      <c r="D45" s="44">
         <f t="shared" si="3"/>
-        <v>10456506.719999999</v>
+        <v>11001484.979049677</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -2656,7 +2670,7 @@
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="10"/>
@@ -2666,20 +2680,20 @@
     </row>
     <row r="47" spans="1:12" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A47" s="68" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="69"/>
       <c r="C47" s="66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D47" s="66"/>
       <c r="E47" s="67"/>
       <c r="F47" s="10"/>
       <c r="G47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
@@ -2688,19 +2702,19 @@
     </row>
     <row r="48" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="E48" s="56" t="s">
         <v>31</v>
-      </c>
-      <c r="E48" s="57" t="s">
-        <v>32</v>
       </c>
       <c r="F48" s="10"/>
       <c r="G48" s="1">
@@ -2716,18 +2730,18 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="37">
+        <v>33</v>
+      </c>
+      <c r="B49" s="36">
         <v>425</v>
       </c>
-      <c r="C49" s="37">
+      <c r="C49" s="36">
         <v>180</v>
       </c>
       <c r="D49" s="1">
         <v>5</v>
       </c>
-      <c r="E49" s="58">
+      <c r="E49" s="57">
         <f>IF(ISERROR((B49-C49)/D49),0,(B49*$H$48-C49*$H$52)/D49)</f>
         <v>1096</v>
       </c>
@@ -2745,18 +2759,18 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="37">
+        <v>34</v>
+      </c>
+      <c r="B50" s="36">
         <v>125</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="36">
         <v>40</v>
       </c>
       <c r="D50" s="1">
         <v>10</v>
       </c>
-      <c r="E50" s="58">
+      <c r="E50" s="57">
         <f>IF(ISERROR((B50-C50)/D50),0,(B50*$H$48-C50*$H$52)/D50)</f>
         <v>244</v>
       </c>
@@ -2774,18 +2788,18 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="B51" s="37">
+        <v>35</v>
+      </c>
+      <c r="B51" s="36">
         <v>66</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="36">
         <v>15</v>
       </c>
       <c r="D51" s="1">
         <v>5</v>
       </c>
-      <c r="E51" s="58">
+      <c r="E51" s="57">
         <f>IF(ISERROR((B51-C51)/D51),0,(B51*$H$48-C51*$H$52)/D51)</f>
         <v>336</v>
       </c>
@@ -2803,18 +2817,18 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="37">
+        <v>36</v>
+      </c>
+      <c r="B52" s="36">
         <v>279</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="36">
         <v>110</v>
       </c>
       <c r="D52" s="1">
         <v>5</v>
       </c>
-      <c r="E52" s="58">
+      <c r="E52" s="57">
         <f>IF(ISERROR((B52-C52)/D52),0,(B52*$H$48-C52*$H$52)/D52)</f>
         <v>824</v>
       </c>
@@ -2832,18 +2846,18 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B53" s="37">
+        <v>37</v>
+      </c>
+      <c r="B53" s="36">
         <v>95</v>
       </c>
-      <c r="C53" s="37">
+      <c r="C53" s="36">
         <v>15</v>
       </c>
       <c r="D53" s="1">
         <v>3</v>
       </c>
-      <c r="E53" s="58">
+      <c r="E53" s="57">
         <f>IF(ISERROR((B53-C53)/D53),0,(B53*$H$48-C53*H50)/D53)</f>
         <v>1001.6666666666666</v>
       </c>
@@ -2857,11 +2871,11 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="36"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="58">
-        <f t="shared" ref="E54:E77" si="4">IF(ISERROR((B54-C54)/D54),0,(B54*$H$48-C54*$H$52)/D54)</f>
+      <c r="E54" s="57">
+        <f t="shared" ref="E54:E77" si="5">IF(ISERROR((B54-C54)/D54),0,(B54*$H$48-C54*$H$52)/D54)</f>
         <v>0</v>
       </c>
       <c r="F54" s="10"/>
@@ -2874,11 +2888,11 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="36"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="58">
-        <f t="shared" si="4"/>
+      <c r="E55" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F55" s="10"/>
@@ -2891,16 +2905,16 @@
     </row>
     <row r="56" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
-      <c r="B56" s="37"/>
-      <c r="C56" s="37"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="36"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="58">
-        <f t="shared" si="4"/>
+      <c r="E56" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H56" s="10"/>
       <c r="I56" s="10"/>
@@ -2910,22 +2924,22 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="37"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="58">
-        <f t="shared" si="4"/>
+      <c r="E57" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H57" s="1">
         <v>16</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
@@ -2933,16 +2947,16 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="58">
-        <f t="shared" si="4"/>
+      <c r="E58" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F58" s="10"/>
       <c r="G58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H58" s="32">
         <v>8</v>
@@ -2954,16 +2968,16 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="58">
-        <f t="shared" si="4"/>
+      <c r="E59" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F59" s="10"/>
       <c r="G59" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H59" s="32">
         <v>22</v>
@@ -2975,16 +2989,16 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="18"/>
-      <c r="B60" s="37"/>
-      <c r="C60" s="37"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="58">
-        <f t="shared" si="4"/>
+      <c r="E60" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F60" s="10"/>
       <c r="G60" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H60" s="32">
         <v>4</v>
@@ -2996,16 +3010,16 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="18"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="36"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="58">
-        <f t="shared" si="4"/>
+      <c r="E61" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F61" s="10"/>
       <c r="G61" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H61" s="32">
         <f>H57*H48*H58*H59*H60</f>
@@ -3018,16 +3032,16 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="18"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="58">
-        <f t="shared" si="4"/>
+      <c r="E62" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F62" s="10"/>
       <c r="G62" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H62" s="32">
         <f>H57*H49*H58*H59*H60</f>
@@ -3040,16 +3054,16 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="18"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="37"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="58">
-        <f t="shared" si="4"/>
+      <c r="E63" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H63" s="32">
         <f>H57*H50*H58*H59*H60</f>
@@ -3062,16 +3076,16 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="18"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="37"/>
+      <c r="B64" s="36"/>
+      <c r="C64" s="36"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="58">
-        <f t="shared" si="4"/>
+      <c r="E64" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H64" s="32">
         <f>H57*H51*H58*H59*H60</f>
@@ -3084,16 +3098,16 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
-      <c r="B65" s="37"/>
-      <c r="C65" s="37"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="58">
-        <f t="shared" si="4"/>
+      <c r="E65" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H65" s="32">
         <f>H57*H52*H58*H59*H60</f>
@@ -3106,22 +3120,22 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="18"/>
-      <c r="B66" s="37"/>
-      <c r="C66" s="37"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="36"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="58">
-        <f t="shared" si="4"/>
+      <c r="E66" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H66" s="1">
         <v>30</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J66" s="10"/>
       <c r="K66" s="10"/>
@@ -3129,22 +3143,22 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="18"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="37"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="58">
-        <f t="shared" si="4"/>
+      <c r="E67" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H67" s="1">
         <v>150</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -3152,22 +3166,22 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="18"/>
-      <c r="B68" s="37"/>
-      <c r="C68" s="37"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="58">
-        <f t="shared" si="4"/>
+      <c r="E68" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H68" s="1">
         <v>88</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
@@ -3175,11 +3189,11 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="18"/>
-      <c r="B69" s="37"/>
-      <c r="C69" s="37"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="36"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="58">
-        <f t="shared" si="4"/>
+      <c r="E69" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F69" s="10"/>
@@ -3192,11 +3206,11 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="18"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="37"/>
+      <c r="B70" s="36"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="58">
-        <f t="shared" si="4"/>
+      <c r="E70" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F70" s="10"/>
@@ -3209,17 +3223,15 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="18"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="37"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="58">
-        <f t="shared" si="4"/>
+      <c r="E71" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F71" s="10"/>
-      <c r="G71" s="31" t="s">
-        <v>68</v>
-      </c>
+      <c r="G71" s="31"/>
       <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
@@ -3228,11 +3240,11 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="18"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="37"/>
+      <c r="B72" s="36"/>
+      <c r="C72" s="36"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="58">
-        <f t="shared" si="4"/>
+      <c r="E72" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F72" s="10"/>
@@ -3245,11 +3257,11 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="18"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="37"/>
+      <c r="B73" s="36"/>
+      <c r="C73" s="36"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="58">
-        <f t="shared" si="4"/>
+      <c r="E73" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F73" s="10"/>
@@ -3262,11 +3274,11 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="18"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="37"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="1"/>
-      <c r="E74" s="58">
-        <f t="shared" si="4"/>
+      <c r="E74" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F74" s="10"/>
@@ -3279,11 +3291,11 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="18"/>
-      <c r="B75" s="37"/>
-      <c r="C75" s="37"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="36"/>
       <c r="D75" s="1"/>
-      <c r="E75" s="58">
-        <f t="shared" si="4"/>
+      <c r="E75" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F75" s="10"/>
@@ -3296,11 +3308,11 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="18"/>
-      <c r="B76" s="37"/>
-      <c r="C76" s="37"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="36"/>
       <c r="D76" s="1"/>
-      <c r="E76" s="58">
-        <f t="shared" si="4"/>
+      <c r="E76" s="57">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F76" s="10"/>
@@ -3312,12 +3324,12 @@
       <c r="L76" s="11"/>
     </row>
     <row r="77" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="53"/>
-      <c r="B77" s="59"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="61">
-        <f t="shared" si="4"/>
+      <c r="A77" s="52"/>
+      <c r="B77" s="58"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="60">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F77" s="10"/>

</xml_diff>

<commit_message>
Integrador al 85%, Rne, FF, Shell de sistemas
</commit_message>
<xml_diff>
--- a/Actividades/Femp03011/Flujo de fondos v1.xlsx
+++ b/Actividades/Femp03011/Flujo de fondos v1.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\HUB\ProyectoFinal2019-\Actividades\Femp03011\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\ProyectoFinal2019-\Actividades\Femp03011\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FF3FBE-A2E1-4D9A-9F5A-2BA4F5F50603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AA0695-29BF-4C67-A523-385CA2D42D52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formula" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tablas Calculadas " sheetId="2" r:id="rId2"/>
     <sheet name="Constantes" sheetId="3" r:id="rId3"/>
     <sheet name="Observaciones" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="164">
-  <si>
-    <t xml:space="preserve">Formula: </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="161">
   <si>
     <r>
       <t>∆V</t>
@@ -297,9 +294,6 @@
     <t>Electricidad</t>
   </si>
   <si>
-    <t>Flujo de fondos</t>
-  </si>
-  <si>
     <t>Instalacion del hardware  (plan economico)</t>
   </si>
   <si>
@@ -576,107 +570,6 @@
   </si>
   <si>
     <t xml:space="preserve">Los costos variables se calculan con todos la sección tributaria, salarial y compra de equipamiento para la realización de la instalación del hardware, variando su valor en el tipo de instalación que se haga     </t>
-  </si>
-  <si>
-    <r>
-      <t>(∆V</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">j </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>- ∆Co</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">j </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>- ∆Am</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">j </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>) * (1-t) + ∆Am</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>j</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> - II</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>+</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="40"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">j </t>
-    </r>
   </si>
   <si>
     <r>
@@ -754,7 +647,7 @@
     <numFmt numFmtId="168" formatCode="_-[$$-2C0A]\ * #,##0.00_-;\-[$$-2C0A]\ * #,##0.00_-;_-[$$-2C0A]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_ [$$-340A]* #,##0.00_ ;_ [$$-340A]* \-#,##0.00_ ;_ [$$-340A]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,39 +750,6 @@
     </font>
     <font>
       <b/>
-      <sz val="40"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="40"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="40"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="40"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="40"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="25"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -914,6 +774,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -921,12 +794,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF3399FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -940,6 +807,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="87">
     <border>
@@ -2063,7 +1936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2124,77 +1997,8 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2223,31 +2027,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2262,17 +2042,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2281,24 +2052,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -2316,6 +2069,150 @@
     <xf numFmtId="168" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2324,156 +2221,137 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="85" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="78" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="86" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="20" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3015,10 +2893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3030,183 +2908,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="182.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="184" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="185"/>
-      <c r="C1" s="185"/>
-      <c r="D1" s="185"/>
-      <c r="E1" s="186"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="124" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="126"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="187"/>
-      <c r="C2" s="187"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="181"/>
-    </row>
-    <row r="3" spans="1:5" ht="57.75" x14ac:dyDescent="0.65">
-      <c r="A3" s="177" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="189" t="s">
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="111"/>
+    </row>
+    <row r="3" spans="1:5" ht="47.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="111"/>
+    </row>
+    <row r="4" spans="1:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="116"/>
+      <c r="E4" s="111"/>
+    </row>
+    <row r="5" spans="1:5" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="C3" s="189"/>
-      <c r="D3" s="189"/>
-      <c r="E3" s="181"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A4" s="178"/>
-      <c r="B4" s="179"/>
-      <c r="C4" s="179"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="181"/>
-    </row>
-    <row r="5" spans="1:5" ht="50.25" x14ac:dyDescent="0.7">
-      <c r="A5" s="180" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="190">
-        <f>(Hoja2!B6-Hoja2!B7-Hoja2!B8)*(1-Hoja2!B9)+Hoja2!B8-Hoja2!B11</f>
+      <c r="B5" s="122"/>
+      <c r="C5" s="117">
+        <f>'Tablas Calculadas '!I20</f>
+        <v>24831184.520133331</v>
+      </c>
+      <c r="D5" s="118"/>
+      <c r="E5" s="111"/>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="123" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="123"/>
+      <c r="C6" s="119">
+        <f>SUM('Tablas Calculadas '!C61:C65)</f>
+        <v>28746102.399999999</v>
+      </c>
+      <c r="D6" s="120"/>
+      <c r="E6" s="111"/>
+    </row>
+    <row r="7" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A7" s="121" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="121"/>
+      <c r="C7" s="119">
+        <f>SUM('Tablas Calculadas '!B61:B65)</f>
+        <v>3267883.6799999997</v>
+      </c>
+      <c r="D7" s="120"/>
+      <c r="E7" s="111"/>
+    </row>
+    <row r="8" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A8" s="121" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="121"/>
+      <c r="C8" s="119">
+        <f>SUM(Constantes!E55:E83)</f>
+        <v>2800.5</v>
+      </c>
+      <c r="D8" s="120"/>
+      <c r="E8" s="111"/>
+    </row>
+    <row r="9" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A9" s="121" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="121"/>
+      <c r="C9" s="195">
+        <f>C5-(C6+C7+C8)</f>
+        <v>-7185602.0598666668</v>
+      </c>
+      <c r="D9" s="196"/>
+      <c r="E9" s="111"/>
+    </row>
+    <row r="10" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A10" s="121" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="121"/>
+      <c r="C10" s="197">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="197"/>
+      <c r="E10" s="111"/>
+    </row>
+    <row r="11" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A11" s="121" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="121"/>
+      <c r="C11" s="195">
+        <f>C9*(1-C10)</f>
+        <v>-5389201.5449000001</v>
+      </c>
+      <c r="D11" s="196"/>
+      <c r="E11" s="111"/>
+    </row>
+    <row r="12" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
+      <c r="A12" s="121" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="121"/>
+      <c r="C12" s="195">
+        <f>SUM(Constantes!E55:E83)</f>
+        <v>2800.5</v>
+      </c>
+      <c r="D12" s="195"/>
+      <c r="E12" s="111"/>
+    </row>
+    <row r="13" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="115" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="115"/>
+      <c r="C13" s="198">
+        <f>'Tablas Calculadas '!B11</f>
+        <v>533080</v>
+      </c>
+      <c r="D13" s="198"/>
+      <c r="E13" s="111"/>
+    </row>
+    <row r="14" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="199" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="199"/>
+      <c r="C14" s="200">
+        <f>C11+C12-C13</f>
         <v>-5919481.0449000001</v>
       </c>
-      <c r="C5" s="190"/>
-      <c r="D5" s="190"/>
-      <c r="E5" s="181"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="188"/>
-      <c r="C6" s="188"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="181"/>
-    </row>
-    <row r="7" spans="1:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="192" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="192"/>
-      <c r="C7" s="192" t="s">
-        <v>163</v>
-      </c>
-      <c r="D7" s="192"/>
-      <c r="E7" s="181"/>
-    </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="195" t="s">
-        <v>153</v>
-      </c>
-      <c r="B8" s="195"/>
-      <c r="C8" s="199">
-        <f>Hoja2!I20</f>
-        <v>24831184.520133331</v>
-      </c>
-      <c r="D8" s="200"/>
-      <c r="E8" s="181"/>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="196" t="s">
-        <v>154</v>
-      </c>
-      <c r="B9" s="196"/>
-      <c r="C9" s="201">
-        <f>SUM(Hoja2!C61:C65)</f>
-        <v>28746102.399999999</v>
-      </c>
-      <c r="D9" s="202"/>
-      <c r="E9" s="181"/>
-    </row>
-    <row r="10" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A10" s="197" t="s">
-        <v>155</v>
-      </c>
-      <c r="B10" s="197"/>
-      <c r="C10" s="201">
-        <f>SUM(Hoja2!B61:B65)</f>
-        <v>3267883.6799999997</v>
-      </c>
-      <c r="D10" s="202"/>
-      <c r="E10" s="181"/>
-    </row>
-    <row r="11" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A11" s="197" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="197"/>
-      <c r="C11" s="201">
-        <f>SUM(Hoja2!E70:E98)</f>
-        <v>2800.5</v>
-      </c>
-      <c r="D11" s="202"/>
-      <c r="E11" s="181"/>
-    </row>
-    <row r="12" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A12" s="197" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="197"/>
-      <c r="C12" s="197"/>
-      <c r="D12" s="197"/>
-      <c r="E12" s="181"/>
-    </row>
-    <row r="13" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A13" s="197" t="s">
-        <v>157</v>
-      </c>
-      <c r="B13" s="197"/>
-      <c r="C13" s="197"/>
-      <c r="D13" s="197"/>
-      <c r="E13" s="181"/>
-    </row>
-    <row r="14" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A14" s="197" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="197"/>
-      <c r="C14" s="197"/>
-      <c r="D14" s="197"/>
-      <c r="E14" s="181"/>
-    </row>
-    <row r="15" spans="1:5" ht="32.25" x14ac:dyDescent="0.5">
-      <c r="A15" s="197" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="197"/>
-      <c r="C15" s="197"/>
-      <c r="D15" s="197"/>
-      <c r="E15" s="181"/>
-    </row>
-    <row r="16" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="198" t="s">
-        <v>161</v>
-      </c>
-      <c r="B16" s="198"/>
-      <c r="C16" s="198"/>
-      <c r="D16" s="198"/>
-      <c r="E16" s="181"/>
-    </row>
-    <row r="17" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="193" t="s">
-        <v>162</v>
-      </c>
-      <c r="B17" s="193"/>
-      <c r="C17" s="194"/>
-      <c r="D17" s="194"/>
-      <c r="E17" s="181"/>
+      <c r="D14" s="201"/>
+      <c r="E14" s="111"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="111"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="111"/>
+    </row>
+    <row r="17" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="111"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="187"/>
-      <c r="E18" s="181"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="111"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="33"/>
       <c r="B19" s="33"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
-      <c r="E19" s="191"/>
+      <c r="E19" s="114"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
@@ -3251,9 +3134,19 @@
       <c r="D28" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
+  <mergeCells count="23">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
@@ -3262,21 +3155,9 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3287,10 +3168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F9F275-8C24-4239-85F2-B9427284E4F8}">
-  <dimension ref="A1:J98"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,178 +3190,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="205.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="182" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="183"/>
-      <c r="C1" s="183"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
-      <c r="F1" s="183"/>
-      <c r="G1" s="183"/>
-      <c r="H1" s="183"/>
-      <c r="I1" s="183"/>
-      <c r="J1" s="183"/>
+      <c r="A1" s="130" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="160" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="161"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="162"/>
+    </row>
+    <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="55"/>
+      <c r="B5" s="152" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101"/>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="74"/>
-      <c r="B5" s="75" t="s">
+      <c r="C5" s="153"/>
+      <c r="D5" s="158" t="s">
         <v>58</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="78"/>
+      <c r="E5" s="159"/>
     </row>
     <row r="6" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="156">
+        <f>'Tablas Calculadas '!I20</f>
+        <v>24831184.520133331</v>
+      </c>
+      <c r="C6" s="157"/>
+      <c r="D6" s="163">
+        <v>0</v>
+      </c>
+      <c r="E6" s="164"/>
+      <c r="F6" s="132" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="146">
-        <f>Hoja2!I20</f>
-        <v>24831184.520133331</v>
-      </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="148">
+      <c r="B7" s="154">
+        <f>SUM('Tablas Calculadas '!B66:C66)</f>
+        <v>32013986.079999998</v>
+      </c>
+      <c r="C7" s="155"/>
+      <c r="D7" s="165">
         <v>0</v>
       </c>
-      <c r="E6" s="149"/>
-      <c r="F6" s="169" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="71" t="s">
+      <c r="E7" s="166"/>
+      <c r="F7" s="133"/>
+    </row>
+    <row r="8" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="154">
+        <f>SUM(Constantes!E55:E83)</f>
+        <v>2800.5</v>
+      </c>
+      <c r="C8" s="155"/>
+      <c r="D8" s="165">
+        <v>0</v>
+      </c>
+      <c r="E8" s="166"/>
+      <c r="F8" s="134"/>
+    </row>
+    <row r="9" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="150">
-        <f>SUM(Hoja2!B66:C66)</f>
-        <v>32013986.079999998</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="70">
-        <v>0</v>
-      </c>
-      <c r="E7" s="151"/>
-      <c r="F7" s="173"/>
-    </row>
-    <row r="8" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="150">
-        <f>SUM(Hoja2!E70:E98)</f>
-        <v>2800.5</v>
-      </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="70">
-        <v>0</v>
-      </c>
-      <c r="E8" s="151"/>
-      <c r="F8" s="170"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="71" t="s">
+      <c r="B9" s="145">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="146"/>
+      <c r="D9" s="146"/>
+      <c r="E9" s="147"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="152">
-        <v>0.25</v>
-      </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="153"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="154" t="s">
+      <c r="B10" s="169" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="170"/>
+      <c r="D10" s="148" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="62" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="155"/>
+      <c r="E10" s="149"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73"/>
-      <c r="B11" s="156">
+      <c r="A11" s="168"/>
+      <c r="B11" s="150">
         <f>D11*Constantes!B26</f>
         <v>533080</v>
       </c>
-      <c r="C11" s="157"/>
-      <c r="D11" s="158">
+      <c r="C11" s="151"/>
+      <c r="D11" s="143">
         <v>13327</v>
       </c>
-      <c r="E11" s="159"/>
+      <c r="E11" s="144"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:10" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="102" t="s">
+      <c r="A14" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="68" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="78" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="135" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="91" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="91" t="s">
-        <v>99</v>
-      </c>
-      <c r="D14" s="91" t="s">
-        <v>100</v>
-      </c>
-      <c r="E14" s="91" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="91" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="91" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" s="109" t="s">
-        <v>55</v>
-      </c>
-      <c r="J14" s="174" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="93"/>
+      <c r="B15" s="70"/>
       <c r="C15" s="27"/>
       <c r="D15" s="47"/>
       <c r="E15" s="47"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="110">
-        <f>B15*Hoja2!E27+C15*Hoja2!E28+F15*Hoja2!E43+G15*Hoja2!E44+Hoja2!E45*H15+D15*Hoja2!E33+E15*Hoja2!E38</f>
+      <c r="I15" s="79">
+        <f>B15*'Tablas Calculadas '!E27+C15*'Tablas Calculadas '!E28+F15*'Tablas Calculadas '!E43+G15*'Tablas Calculadas '!E44+'Tablas Calculadas '!E45*H15+D15*'Tablas Calculadas '!E33+E15*'Tablas Calculadas '!E38</f>
         <v>0</v>
       </c>
-      <c r="J15" s="175"/>
+      <c r="J15" s="136"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="97" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="94">
+      <c r="A16" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="71">
         <v>1</v>
       </c>
       <c r="C16" s="1">
@@ -3495,17 +3376,17 @@
         <v>1</v>
       </c>
       <c r="H16" s="3"/>
-      <c r="I16" s="111">
-        <f>B16*Hoja2!E27+C16*Hoja2!E29+F16*Hoja2!E46+G16*Hoja2!E47+Hoja2!E48*H16+D16*Hoja2!E34+E16*Hoja2!E39</f>
+      <c r="I16" s="80">
+        <f>B16*'Tablas Calculadas '!E27+C16*'Tablas Calculadas '!E29+F16*'Tablas Calculadas '!E46+G16*'Tablas Calculadas '!E47+'Tablas Calculadas '!E48*H16+D16*'Tablas Calculadas '!E34+E16*'Tablas Calculadas '!E39</f>
         <v>10793581.323733332</v>
       </c>
-      <c r="J16" s="175"/>
+      <c r="J16" s="136"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="94"/>
+      <c r="A17" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="71"/>
       <c r="C17" s="1">
         <v>5</v>
       </c>
@@ -3518,17 +3399,17 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="111">
-        <f>B17*Hoja2!E27+C17*Hoja2!E30+F17*Hoja2!E49+G17*Hoja2!E50+H17*Hoja2!E51+D17*Hoja2!E35+E17*Hoja2!E40</f>
+      <c r="I17" s="80">
+        <f>B17*'Tablas Calculadas '!E27+C17*'Tablas Calculadas '!E30+F17*'Tablas Calculadas '!E49+G17*'Tablas Calculadas '!E50+H17*'Tablas Calculadas '!E51+D17*'Tablas Calculadas '!E35+E17*'Tablas Calculadas '!E40</f>
         <v>2520097.3745333333</v>
       </c>
-      <c r="J17" s="175"/>
+      <c r="J17" s="136"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="94"/>
+      <c r="A18" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="71"/>
       <c r="C18" s="1">
         <v>4</v>
       </c>
@@ -3541,17 +3422,17 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="110">
-        <f>B18*Hoja2!E27+C18*Hoja2!E31+F18*Hoja2!E52+Hoja2!E53*G18+H18*Hoja2!E54+D18*Hoja2!E36+E18*Hoja2!E41</f>
+      <c r="I18" s="79">
+        <f>B18*'Tablas Calculadas '!E27+C18*'Tablas Calculadas '!E31+F18*'Tablas Calculadas '!E52+'Tablas Calculadas '!E53*G18+H18*'Tablas Calculadas '!E54+D18*'Tablas Calculadas '!E36+E18*'Tablas Calculadas '!E41</f>
         <v>3098812.4458666667</v>
       </c>
-      <c r="J18" s="175"/>
+      <c r="J18" s="136"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="98" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="95"/>
+      <c r="A19" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="72"/>
       <c r="C19" s="1">
         <v>6</v>
       </c>
@@ -3564,105 +3445,105 @@
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
       <c r="H19" s="21"/>
-      <c r="I19" s="112">
-        <f>B19*Hoja2!E27+C19*Hoja2!E32+F19*Hoja2!E55+Hoja2!E56*G19+H19*Hoja2!E57+D19*Hoja2!E37+E19*Hoja2!E42</f>
+      <c r="I19" s="81">
+        <f>B19*'Tablas Calculadas '!E27+C19*'Tablas Calculadas '!E32+F19*'Tablas Calculadas '!E55+'Tablas Calculadas '!E56*G19+H19*'Tablas Calculadas '!E57+D19*'Tablas Calculadas '!E37+E19*'Tablas Calculadas '!E42</f>
         <v>8418693.3760000002</v>
       </c>
-      <c r="J19" s="175"/>
+      <c r="J19" s="136"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="34">
-        <f>SUM(B15:B19)*Hoja2!E27</f>
+        <f>SUM(B15:B19)*'Tablas Calculadas '!E27</f>
         <v>3321612</v>
       </c>
       <c r="C20" s="34">
-        <f>C15*Hoja2!E28+C16*Hoja2!E29+C17*Hoja2!E30+C18*Hoja2!E31+C19*Hoja2!E32</f>
+        <f>C15*'Tablas Calculadas '!E28+C16*'Tablas Calculadas '!E29+C17*'Tablas Calculadas '!E30+C18*'Tablas Calculadas '!E31+C19*'Tablas Calculadas '!E32</f>
         <v>2496087.8833333333</v>
       </c>
       <c r="D20" s="34">
-        <f>D15*Hoja2!E33+D16*Hoja2!E34+D17*Hoja2!E35+D18*Hoja2!E36+D19*Hoja2!E37</f>
+        <f>D15*'Tablas Calculadas '!E33+D16*'Tablas Calculadas '!E34+D17*'Tablas Calculadas '!E35+D18*'Tablas Calculadas '!E36+D19*'Tablas Calculadas '!E37</f>
         <v>5672962.7552000005</v>
       </c>
       <c r="E20" s="49">
-        <f>E15*Hoja2!E38+E16*Hoja2!E39+E17*Hoja2!E40+E18*Hoja2!E41+E19*Hoja2!E42</f>
+        <f>E15*'Tablas Calculadas '!E38+E16*'Tablas Calculadas '!E39+E17*'Tablas Calculadas '!E40+E18*'Tablas Calculadas '!E41+E19*'Tablas Calculadas '!E42</f>
         <v>7703546.4576000003</v>
       </c>
       <c r="F20" s="49">
-        <f>F15*Hoja2!E43+F16*Hoja2!E46+F17*Hoja2!E49+F18*Hoja2!E52+F19*Hoja2!E55</f>
+        <f>F15*'Tablas Calculadas '!E43+F16*'Tablas Calculadas '!E46+F17*'Tablas Calculadas '!E49+F18*'Tablas Calculadas '!E52+F19*'Tablas Calculadas '!E55</f>
         <v>0</v>
       </c>
       <c r="G20" s="49">
-        <f>G15*Hoja2!E44+G16*Hoja2!E47+G17*Hoja2!E50+G18*Hoja2!E53+G19*Hoja2!E56</f>
+        <f>G15*'Tablas Calculadas '!E44+G16*'Tablas Calculadas '!E47+G17*'Tablas Calculadas '!E50+G18*'Tablas Calculadas '!E53+G19*'Tablas Calculadas '!E56</f>
         <v>5636975.4239999996</v>
       </c>
       <c r="H20" s="49">
-        <f>H15*Hoja2!E45+H16*Hoja2!E48+H17*Hoja2!E51+H18*Hoja2!E54+H19*Hoja2!E57</f>
+        <f>H15*'Tablas Calculadas '!E45+H16*'Tablas Calculadas '!E48+H17*'Tablas Calculadas '!E51+H18*'Tablas Calculadas '!E54+H19*'Tablas Calculadas '!E57</f>
         <v>0</v>
       </c>
-      <c r="I20" s="113">
+      <c r="I20" s="82">
         <f>SUM(I15:I19)</f>
         <v>24831184.520133331</v>
       </c>
-      <c r="J20" s="176"/>
+      <c r="J20" s="137"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="139"/>
+      <c r="C25" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="104"/>
-      <c r="C25" s="105" t="s">
+      <c r="D25" s="141"/>
+      <c r="E25" s="142"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="77" t="s">
+        <v>149</v>
+      </c>
+      <c r="C26" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="106"/>
-      <c r="E25" s="107"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="91" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="108" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="91" t="s">
+      <c r="D26" s="68" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="92" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="82" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="79">
+      <c r="A27" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="56">
         <f>(Constantes!C19*(1+((Constantes!D19/100)*0))+ Constantes!C20*(1+((Constantes!D20/100)*0)) + Constantes!C21*(1+((Constantes!D21/100)*0)))*Constantes!B26*7</f>
         <v>281960</v>
       </c>
-      <c r="C27" s="79">
-        <f>((Hoja2!C62-C47)/12)*7</f>
+      <c r="C27" s="56">
+        <f>(('Tablas Calculadas '!C62-C47)/12)*7</f>
         <v>2375329.6</v>
       </c>
-      <c r="D27" s="80">
+      <c r="D27" s="57">
         <v>25</v>
       </c>
-      <c r="E27" s="81">
-        <f>SUM(B27:C27)*(1+(D27/100))</f>
+      <c r="E27" s="58">
+        <f t="shared" ref="E27:E57" si="0">SUM(B27:C27)*(1+(D27/100))</f>
         <v>3321612</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="87" t="s">
-        <v>114</v>
-      </c>
-      <c r="B28" s="83">
-        <f>(Hoja2!B61/(12*30))*(Constantes!$C$10+2)</f>
+      <c r="A28" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="60">
+        <f>('Tablas Calculadas '!B61/(12*30))*(Constantes!$C$10+2)</f>
         <v>13426.666666666668</v>
       </c>
       <c r="C28" s="28">
@@ -3673,16 +3554,16 @@
         <v>25</v>
       </c>
       <c r="E28" s="32">
-        <f>SUM(B28:C28)*(1+(D28/100))</f>
+        <f t="shared" si="0"/>
         <v>93583.333333333343</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="88" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="83">
-        <f>(Hoja2!B62/(12*30))*(Constantes!$C$10+2)</f>
+      <c r="A29" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="60">
+        <f>('Tablas Calculadas '!B62/(12*30))*(Constantes!$C$10+2)</f>
         <v>16246.586666666662</v>
       </c>
       <c r="C29" s="28">
@@ -3693,16 +3574,16 @@
         <v>25</v>
       </c>
       <c r="E29" s="22">
-        <f>SUM(B29:C29)*(1+(D29/100))</f>
+        <f t="shared" si="0"/>
         <v>108628.23333333334</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="88" t="s">
-        <v>116</v>
-      </c>
-      <c r="B30" s="83">
-        <f>(Hoja2!B63/(12*30))*(Constantes!$C$10+2)</f>
+      <c r="A30" s="65" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="60">
+        <f>('Tablas Calculadas '!B63/(12*30))*(Constantes!$C$10+2)</f>
         <v>18718.893333333333</v>
       </c>
       <c r="C30" s="28">
@@ -3713,16 +3594,16 @@
         <v>25</v>
       </c>
       <c r="E30" s="22">
-        <f>SUM(B30:C30)*(1+(D30/100))</f>
+        <f t="shared" si="0"/>
         <v>125158.61666666667</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="88" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="83">
-        <f>(Hoja2!B64/(12*30))*(Constantes!$C$10+2)</f>
+      <c r="A31" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="60">
+        <f>('Tablas Calculadas '!B64/(12*30))*(Constantes!$C$10+2)</f>
         <v>19778.453333333335</v>
       </c>
       <c r="C31" s="28">
@@ -3733,16 +3614,16 @@
         <v>25</v>
       </c>
       <c r="E31" s="22">
-        <f>SUM(B31:C31)*(1+(D31/100))</f>
+        <f t="shared" si="0"/>
         <v>132243.06666666668</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="88" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="84">
-        <f>(Hoja2!B65/(12*30))*(Constantes!$C$10+2)</f>
+      <c r="A32" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B32" s="61">
+        <f>('Tablas Calculadas '!B65/(12*30))*(Constantes!$C$10+2)</f>
         <v>22603.946666666667</v>
       </c>
       <c r="C32" s="26">
@@ -3753,16 +3634,16 @@
         <v>25</v>
       </c>
       <c r="E32" s="24">
-        <f>SUM(B32:C32)*(1+(D32/100))</f>
+        <f t="shared" si="0"/>
         <v>151134.93333333335</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="B33" s="83">
-        <f>(Hoja2!B61/(12*30))*(Constantes!$C$11+2)</f>
+      <c r="A33" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="60">
+        <f>('Tablas Calculadas '!B61/(12*30))*(Constantes!$C$11+2)</f>
         <v>29538.666666666668</v>
       </c>
       <c r="C33" s="28">
@@ -3773,16 +3654,16 @@
         <v>20</v>
       </c>
       <c r="E33" s="32">
-        <f>SUM(B33:C33)*(1+(D33/100))</f>
+        <f t="shared" si="0"/>
         <v>404086.4</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="89" t="s">
-        <v>120</v>
-      </c>
-      <c r="B34" s="83">
-        <f>(Hoja2!B62/(12*30))*(Constantes!$C$11+2)</f>
+      <c r="A34" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="60">
+        <f>('Tablas Calculadas '!B62/(12*30))*(Constantes!$C$11+2)</f>
         <v>35742.490666666657</v>
       </c>
       <c r="C34" s="28">
@@ -3793,16 +3674,16 @@
         <v>20</v>
       </c>
       <c r="E34" s="22">
-        <f>SUM(B34:C34)*(1+(D34/100))</f>
+        <f t="shared" si="0"/>
         <v>466826.98879999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="B35" s="83">
-        <f>(Hoja2!B63/(12*30))*(Constantes!$C$11+2)</f>
+      <c r="A35" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="60">
+        <f>('Tablas Calculadas '!B63/(12*30))*(Constantes!$C$11+2)</f>
         <v>41181.565333333339</v>
       </c>
       <c r="C35" s="28">
@@ -3813,16 +3694,16 @@
         <v>20</v>
       </c>
       <c r="E35" s="22">
-        <f>SUM(B35:C35)*(1+(D35/100))</f>
+        <f t="shared" si="0"/>
         <v>537865.87839999993</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="B36" s="83">
-        <f>(Hoja2!B64/(12*30))*(Constantes!$C$11+2)</f>
+      <c r="A36" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36" s="60">
+        <f>('Tablas Calculadas '!B64/(12*30))*(Constantes!$C$11+2)</f>
         <v>43512.597333333339</v>
       </c>
       <c r="C36" s="28">
@@ -3833,16 +3714,16 @@
         <v>20</v>
       </c>
       <c r="E36" s="22">
-        <f>SUM(B36:C36)*(1+(D36/100))</f>
+        <f t="shared" si="0"/>
         <v>568311.11679999996</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="89" t="s">
-        <v>123</v>
-      </c>
-      <c r="B37" s="84">
-        <f>(Hoja2!B65/(12*30))*(Constantes!$C$11+2)</f>
+      <c r="A37" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B37" s="61">
+        <f>('Tablas Calculadas '!B65/(12*30))*(Constantes!$C$11+2)</f>
         <v>49728.682666666668</v>
       </c>
       <c r="C37" s="26">
@@ -3853,16 +3734,16 @@
         <v>20</v>
       </c>
       <c r="E37" s="24">
-        <f>SUM(B37:C37)*(1+(D37/100))</f>
+        <f t="shared" si="0"/>
         <v>649498.4192</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="89" t="s">
-        <v>124</v>
-      </c>
-      <c r="B38" s="83">
-        <f>(Hoja2!B61/(12*30))*(Constantes!$C$12+2)</f>
+      <c r="A38" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="60">
+        <f>('Tablas Calculadas '!B61/(12*30))*(Constantes!$C$12+2)</f>
         <v>32224</v>
       </c>
       <c r="C38" s="28">
@@ -3873,16 +3754,16 @@
         <v>20</v>
       </c>
       <c r="E38" s="32">
-        <f>SUM(B38:C38)*(1+(D38/100))</f>
+        <f t="shared" si="0"/>
         <v>1021708.7999999999</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="89" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="83">
-        <f>(Hoja2!B62/(12*30))*(Constantes!$C$12+2)</f>
+      <c r="A39" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" s="60">
+        <f>('Tablas Calculadas '!B62/(12*30))*(Constantes!$C$12+2)</f>
         <v>38991.80799999999</v>
       </c>
       <c r="C39" s="25">
@@ -3893,16 +3774,16 @@
         <v>20</v>
       </c>
       <c r="E39" s="22">
-        <f>SUM(B39:C39)*(1+(D39/100))</f>
+        <f t="shared" si="0"/>
         <v>1177286.1695999999</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="89" t="s">
-        <v>126</v>
-      </c>
-      <c r="B40" s="83">
-        <f>(Hoja2!B63/(12*30))*(Constantes!$C$12+2)</f>
+      <c r="A40" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="60">
+        <f>('Tablas Calculadas '!B63/(12*30))*(Constantes!$C$12+2)</f>
         <v>44925.344000000005</v>
       </c>
       <c r="C40" s="25">
@@ -3913,16 +3794,16 @@
         <v>20</v>
       </c>
       <c r="E40" s="22">
-        <f>SUM(B40:C40)*(1+(D40/100))</f>
+        <f t="shared" si="0"/>
         <v>1356438.4128</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="89" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="83">
-        <f>(Hoja2!B64/(12*30))*(Constantes!$C$12+2)</f>
+      <c r="A41" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="60">
+        <f>('Tablas Calculadas '!B64/(12*30))*(Constantes!$C$12+2)</f>
         <v>47468.288</v>
       </c>
       <c r="C41" s="25">
@@ -3933,16 +3814,16 @@
         <v>20</v>
       </c>
       <c r="E41" s="22">
-        <f>SUM(B41:C41)*(1+(D41/100))</f>
+        <f t="shared" si="0"/>
         <v>1433217.9456</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="85">
-        <f>(Hoja2!B65/(12*30))*(Constantes!$C$12+2)</f>
+      <c r="A42" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="62">
+        <f>('Tablas Calculadas '!B65/(12*30))*(Constantes!$C$12+2)</f>
         <v>54249.471999999994</v>
       </c>
       <c r="C42" s="42">
@@ -3953,16 +3834,16 @@
         <v>20</v>
       </c>
       <c r="E42" s="44">
-        <f>SUM(B42:C42)*(1+(D42/100))</f>
+        <f t="shared" si="0"/>
         <v>1637963.3663999999</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" s="83">
-        <f>Hoja2!B61/12*2</f>
+      <c r="A43" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="60">
+        <f>'Tablas Calculadas '!B61/12*2</f>
         <v>80560</v>
       </c>
       <c r="C43" s="28">
@@ -3973,16 +3854,16 @@
         <v>20</v>
       </c>
       <c r="E43" s="30">
-        <f>SUM(B43:C43)*(1+(D43/100))</f>
+        <f t="shared" si="0"/>
         <v>2496672</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="86">
-        <f>Hoja2!B61/12*2</f>
+        <v>64</v>
+      </c>
+      <c r="B44" s="63">
+        <f>'Tablas Calculadas '!B61/12*2</f>
         <v>80560</v>
       </c>
       <c r="C44" s="25">
@@ -3993,16 +3874,16 @@
         <v>20</v>
       </c>
       <c r="E44" s="23">
-        <f>SUM(B44:C44)*(1+(D44/100))</f>
+        <f t="shared" si="0"/>
         <v>4896672</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B45" s="84">
-        <f>Hoja2!B61/12*2</f>
+        <v>81</v>
+      </c>
+      <c r="B45" s="61">
+        <f>'Tablas Calculadas '!B61/12*2</f>
         <v>80560</v>
       </c>
       <c r="C45" s="26">
@@ -4013,16 +3894,16 @@
         <v>20</v>
       </c>
       <c r="E45" s="24">
-        <f>SUM(B45:C45)*(1+(D45/100))</f>
+        <f t="shared" si="0"/>
         <v>7296672</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="90" t="s">
-        <v>84</v>
-      </c>
-      <c r="B46" s="83">
-        <f>Hoja2!B62/12*2</f>
+      <c r="A46" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="60">
+        <f>'Tablas Calculadas '!B62/12*2</f>
         <v>97479.519999999975</v>
       </c>
       <c r="C46" s="28">
@@ -4033,16 +3914,16 @@
         <v>20</v>
       </c>
       <c r="E46" s="23">
-        <f>SUM(B46:C46)*(1+(D46/100))</f>
+        <f t="shared" si="0"/>
         <v>2876975.4240000001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="86">
-        <f>Hoja2!B62/12*2</f>
+        <v>65</v>
+      </c>
+      <c r="B47" s="63">
+        <f>'Tablas Calculadas '!B62/12*2</f>
         <v>97479.519999999975</v>
       </c>
       <c r="C47" s="25">
@@ -4053,16 +3934,16 @@
         <v>20</v>
       </c>
       <c r="E47" s="23">
-        <f>SUM(B47:C47)*(1+(D47/100))</f>
+        <f t="shared" si="0"/>
         <v>5636975.4239999996</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="84">
-        <f>Hoja2!B62/12*2</f>
+        <v>84</v>
+      </c>
+      <c r="B48" s="61">
+        <f>'Tablas Calculadas '!B62/12*2</f>
         <v>97479.519999999975</v>
       </c>
       <c r="C48" s="26">
@@ -4073,16 +3954,16 @@
         <v>20</v>
       </c>
       <c r="E48" s="24">
-        <f>SUM(B48:C48)*(1+(D48/100))</f>
+        <f t="shared" si="0"/>
         <v>8396975.4239999987</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="90" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="83">
-        <f>Hoja2!$B$63/12*2</f>
+      <c r="A49" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="60">
+        <f>'Tablas Calculadas '!$B$63/12*2</f>
         <v>112313.36</v>
       </c>
       <c r="C49" s="28">
@@ -4093,16 +3974,16 @@
         <v>20</v>
       </c>
       <c r="E49" s="23">
-        <f>SUM(B49:C49)*(1+(D49/100))</f>
+        <f t="shared" si="0"/>
         <v>3314776.0319999997</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B50" s="86">
-        <f>Hoja2!$B$63/12*2</f>
+        <v>66</v>
+      </c>
+      <c r="B50" s="63">
+        <f>'Tablas Calculadas '!$B$63/12*2</f>
         <v>112313.36</v>
       </c>
       <c r="C50" s="25">
@@ -4113,16 +3994,16 @@
         <v>20</v>
       </c>
       <c r="E50" s="23">
-        <f>SUM(B50:C50)*(1+(D50/100))</f>
+        <f t="shared" si="0"/>
         <v>6494776.0320000006</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="84">
-        <f>Hoja2!$B$63/12*2</f>
+        <v>86</v>
+      </c>
+      <c r="B51" s="61">
+        <f>'Tablas Calculadas '!$B$63/12*2</f>
         <v>112313.36</v>
       </c>
       <c r="C51" s="26">
@@ -4133,16 +4014,16 @@
         <v>20</v>
       </c>
       <c r="E51" s="24">
-        <f>SUM(B51:C51)*(1+(D51/100))</f>
+        <f t="shared" si="0"/>
         <v>9674776.0319999997</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="90" t="s">
-        <v>69</v>
-      </c>
-      <c r="B52" s="83">
-        <f>Hoja2!$B$64/12*2</f>
+      <c r="A52" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="60">
+        <f>'Tablas Calculadas '!$B$64/12*2</f>
         <v>118670.72000000002</v>
       </c>
       <c r="C52" s="28">
@@ -4153,16 +4034,16 @@
         <v>20</v>
       </c>
       <c r="E52" s="23">
-        <f>SUM(B52:C52)*(1+(D52/100))</f>
+        <f t="shared" si="0"/>
         <v>3502404.8640000001</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B53" s="86">
-        <f>Hoja2!$B$64/12*2</f>
+        <v>87</v>
+      </c>
+      <c r="B53" s="63">
+        <f>'Tablas Calculadas '!$B$64/12*2</f>
         <v>118670.72000000002</v>
       </c>
       <c r="C53" s="25">
@@ -4173,16 +4054,16 @@
         <v>20</v>
       </c>
       <c r="E53" s="23">
-        <f>SUM(B53:C53)*(1+(D53/100))</f>
+        <f t="shared" si="0"/>
         <v>6862404.8639999991</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="84">
-        <f>Hoja2!$B$64/12*2</f>
+        <v>88</v>
+      </c>
+      <c r="B54" s="61">
+        <f>'Tablas Calculadas '!$B$64/12*2</f>
         <v>118670.72000000002</v>
       </c>
       <c r="C54" s="26">
@@ -4193,16 +4074,16 @@
         <v>20</v>
       </c>
       <c r="E54" s="24">
-        <f>SUM(B54:C54)*(1+(D54/100))</f>
+        <f t="shared" si="0"/>
         <v>10222404.864</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="B55" s="83">
-        <f>Hoja2!$B$65/12*2</f>
+      <c r="A55" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="60">
+        <f>'Tablas Calculadas '!$B$65/12*2</f>
         <v>135623.67999999999</v>
       </c>
       <c r="C55" s="28">
@@ -4213,16 +4094,16 @@
         <v>20</v>
       </c>
       <c r="E55" s="23">
-        <f>SUM(B55:C55)*(1+(D55/100))</f>
+        <f t="shared" si="0"/>
         <v>4002748.4160000002</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="B56" s="86">
-        <f>Hoja2!$B$65/12*2</f>
+        <v>89</v>
+      </c>
+      <c r="B56" s="63">
+        <f>'Tablas Calculadas '!$B$65/12*2</f>
         <v>135623.67999999999</v>
       </c>
       <c r="C56" s="25">
@@ -4233,16 +4114,16 @@
         <v>20</v>
       </c>
       <c r="E56" s="23">
-        <f>SUM(B56:C56)*(1+(D56/100))</f>
+        <f t="shared" si="0"/>
         <v>7842748.4159999993</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B57" s="84">
-        <f>Hoja2!$B$65/12*2</f>
+        <v>90</v>
+      </c>
+      <c r="B57" s="61">
+        <f>'Tablas Calculadas '!$B$65/12*2</f>
         <v>135623.67999999999</v>
       </c>
       <c r="C57" s="26">
@@ -4253,115 +4134,115 @@
         <v>20</v>
       </c>
       <c r="E57" s="24">
-        <f>SUM(B57:C57)*(1+(D57/100))</f>
+        <f t="shared" si="0"/>
         <v>11682748.415999999</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="102" t="s">
+      <c r="A60" s="76" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="102" t="s">
-        <v>18</v>
-      </c>
-      <c r="C60" s="102" t="s">
-        <v>148</v>
-      </c>
-      <c r="D60" s="102" t="s">
-        <v>54</v>
+      <c r="C60" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" s="76" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="96" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="86">
+      <c r="A61" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="63">
         <f>(Constantes!C19*(1+((Constantes!D19/100)*0))+ Constantes!C20*(1+((Constantes!D20/100)*0)) + Constantes!C21*(1+((Constantes!D21/100)*0)))*Constantes!B26*12</f>
         <v>483360</v>
       </c>
       <c r="C61" s="25">
-        <f>Constantes!B40*12+(Constantes!B45*Constantes!B26+Constantes!B46*Constantes!B26+Constantes!B47*Constantes!B26)*12 +Hoja2!F15*Hoja2!C43+Hoja2!G15*Hoja2!C44+Hoja2!H15*Hoja2!C45 + Constantes!B54</f>
+        <f>Constantes!B40*12+(Constantes!B45*Constantes!B26+Constantes!B46*Constantes!B26+Constantes!B47*Constantes!B26)*12 +'Tablas Calculadas '!F15*'Tablas Calculadas '!C43+'Tablas Calculadas '!G15*'Tablas Calculadas '!C44+'Tablas Calculadas '!H15*'Tablas Calculadas '!C45 + 'Tablas Calculadas '!B72</f>
         <v>3540863.9999999995</v>
       </c>
       <c r="D61" s="36">
-        <f>SUM(B61:C61)</f>
+        <f t="shared" ref="D61:D66" si="1">SUM(B61:C61)</f>
         <v>4024223.9999999995</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="97" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="86">
+      <c r="A62" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="63">
         <f>(((Constantes!$C$19*(1+((Constantes!$D$19/100)*1)))+ (Constantes!$C$20*(1+((Constantes!$D$20/100)*1))) + (Constantes!$C$21*(1+((Constantes!$D$21/100)*1))))*Constantes!B27*12)*((1+Constantes!$C$14)^1)</f>
         <v>584877.11999999988</v>
       </c>
       <c r="C62" s="25">
-        <f>(Constantes!B41*12+(Constantes!$B$45*Constantes!B27+Constantes!$B$46*Constantes!B27+Constantes!B47*Constantes!B27)*12) +Hoja2!F16*Hoja2!C46+Hoja2!G16*Hoja2!C47+Hoja2!H16*Hoja2!C48 +Constantes!B55</f>
+        <f>(Constantes!B41*12+(Constantes!$B$45*Constantes!B27+Constantes!$B$46*Constantes!B27+Constantes!B47*Constantes!B27)*12) +'Tablas Calculadas '!F16*'Tablas Calculadas '!C46+'Tablas Calculadas '!G16*'Tablas Calculadas '!C47+'Tablas Calculadas '!H16*'Tablas Calculadas '!C48 +'Tablas Calculadas '!B73</f>
         <v>8671993.5999999996</v>
       </c>
       <c r="D62" s="36">
-        <f>SUM(B62:C62)</f>
+        <f t="shared" si="1"/>
         <v>9256870.7199999988</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="97" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="86">
+      <c r="A63" s="74" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="63">
         <f>(((Constantes!$C$19*(1+((Constantes!$D$19/100)*1)))+ (Constantes!$C$20*(1+((Constantes!$D$20/100)*1))) + (Constantes!$C$21*(1+((Constantes!$D$21/100)*1))))*Constantes!B28*12)*((1+Constantes!$C$14)^2)</f>
         <v>673880.16</v>
       </c>
       <c r="C63" s="25">
-        <f>(Constantes!B42*12+(Constantes!$B$45*Constantes!B28+Constantes!$B$46*Constantes!B28+Constantes!B47*Constantes!B28)*12) +(Hoja2!F17*Hoja2!C49+Hoja2!G17*Hoja2!C50+Hoja2!H17*Hoja2!C51) +Constantes!B56</f>
+        <f>(Constantes!B42*12+(Constantes!$B$45*Constantes!B28+Constantes!$B$46*Constantes!B28+Constantes!B47*Constantes!B28)*12) +('Tablas Calculadas '!F17*'Tablas Calculadas '!C49+'Tablas Calculadas '!G17*'Tablas Calculadas '!C50+'Tablas Calculadas '!H17*'Tablas Calculadas '!C51) +'Tablas Calculadas '!B74</f>
         <v>4935868.8</v>
       </c>
       <c r="D63" s="36">
-        <f>SUM(B63:C63)</f>
+        <f t="shared" si="1"/>
         <v>5609748.96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="97" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64" s="86">
+      <c r="A64" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="B64" s="63">
         <f>(((Constantes!$C$19*(1+((Constantes!$D$19/100)*1)))+ (Constantes!$C$20*(1+((Constantes!$D$20/100)*1))) + (Constantes!$C$21*(1+((Constantes!$D$21/100)*1))))*Constantes!B29*12)*((1+Constantes!$C$14)^3)</f>
         <v>712024.32000000007</v>
       </c>
       <c r="C64" s="25">
-        <f>(Constantes!B43*12+(Constantes!$B$45*Constantes!B29+Constantes!$B$46*Constantes!B29)*12)+(Hoja2!F18*Hoja2!C52+Hoja2!G18*Hoja2!C53+Hoja2!H18*Hoja2!C54) +Constantes!B57</f>
+        <f>(Constantes!B43*12+(Constantes!$B$45*Constantes!B29+Constantes!$B$46*Constantes!B29)*12)+('Tablas Calculadas '!F18*'Tablas Calculadas '!C52+'Tablas Calculadas '!G18*'Tablas Calculadas '!C53+'Tablas Calculadas '!H18*'Tablas Calculadas '!C54) +'Tablas Calculadas '!B75</f>
         <v>5047257.5999999996</v>
       </c>
       <c r="D64" s="36">
-        <f>SUM(B64:C64)</f>
+        <f t="shared" si="1"/>
         <v>5759281.9199999999</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="97" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="86">
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="63">
         <f>(((Constantes!$C$19*(1+((Constantes!$D$19/100)*1)))+ (Constantes!$C$20*(1+((Constantes!$D$20/100)*1))) + (Constantes!$C$21*(1+((Constantes!$D$21/100)*1))))*Constantes!B30*12)*((1+Constantes!$C$14)^4)</f>
         <v>813742.07999999996</v>
       </c>
       <c r="C65" s="25">
-        <f>(Constantes!B44*12+(Constantes!$B$45*Constantes!B30+Constantes!$B$46*Constantes!B30+Constantes!B47*Constantes!B30)*12)+(Hoja2!F19*Hoja2!C55+Hoja2!G19*Hoja2!C56+Hoja2!H19*Hoja2!C57) +Constantes!B58</f>
+        <f>(Constantes!B44*12+(Constantes!$B$45*Constantes!B30+Constantes!$B$46*Constantes!B30+Constantes!B47*Constantes!B30)*12)+('Tablas Calculadas '!F19*'Tablas Calculadas '!C55+'Tablas Calculadas '!G19*'Tablas Calculadas '!C56+'Tablas Calculadas '!H19*'Tablas Calculadas '!C57) +'Tablas Calculadas '!B76</f>
         <v>6550118.3999999994</v>
       </c>
       <c r="D65" s="36">
-        <f>SUM(B65:C65)</f>
+        <f t="shared" si="1"/>
         <v>7363860.4799999995</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="161" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="160">
+    <row r="66" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="106">
         <f>SUM(B61:B65)</f>
         <v>3267883.6799999997</v>
       </c>
@@ -4370,373 +4251,79 @@
         <v>28746102.399999999</v>
       </c>
       <c r="D66" s="35">
-        <f>SUM(B66:C66)</f>
+        <f t="shared" si="1"/>
         <v>32013986.079999998</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="116" t="s">
-        <v>41</v>
-      </c>
-      <c r="B68" s="117"/>
-      <c r="C68" s="116" t="s">
-        <v>19</v>
-      </c>
-      <c r="D68" s="118"/>
-      <c r="E68" s="117"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C69" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E69" s="16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B70" s="12">
-        <v>425</v>
-      </c>
-      <c r="C70" s="12">
-        <v>180</v>
-      </c>
-      <c r="D70" s="1">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="160" t="s">
+        <v>103</v>
+      </c>
+      <c r="B71" s="162"/>
+      <c r="C71" s="109" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="17">
-        <f>IF(ISERROR((B70-C70)/D70),0,(B70*Constantes!$B$26-C70*Constantes!$B$30)/D70)</f>
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B71" s="12">
-        <v>125</v>
-      </c>
-      <c r="C71" s="12">
-        <v>40</v>
-      </c>
-      <c r="D71" s="1">
-        <v>10</v>
-      </c>
-      <c r="E71" s="17">
-        <f>IF(ISERROR((B71-C71)/D71),0,(B71*Constantes!$B$26-C71*Constantes!$B$30)/D71)</f>
-        <v>244</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B72" s="12">
-        <v>66</v>
-      </c>
-      <c r="C72" s="12">
-        <v>15</v>
-      </c>
-      <c r="D72" s="1">
-        <v>5</v>
-      </c>
-      <c r="E72" s="17">
-        <f>IF(ISERROR((B72-C72)/D72),0,(B72*Constantes!$B$26-C72*Constantes!$B$30)/D72)</f>
-        <v>336</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B73" s="12">
-        <v>279</v>
-      </c>
-      <c r="C73" s="12">
-        <v>110</v>
-      </c>
-      <c r="D73" s="1">
-        <v>5</v>
-      </c>
-      <c r="E73" s="17">
-        <f>IF(ISERROR((B73-C73)/D73),0,(B73*Constantes!$B$26-C73*Constantes!$B$30)/D73)</f>
-        <v>824</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B74" s="12">
-        <v>95</v>
-      </c>
-      <c r="C74" s="12">
-        <v>15</v>
-      </c>
-      <c r="D74" s="1">
-        <v>10</v>
-      </c>
-      <c r="E74" s="17">
-        <f>IF(ISERROR((B74-C74)/D74),0,(B74*Constantes!$B$26-C74*Constantes!B28)/D74)</f>
-        <v>300.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="17">
-        <f>IF(ISERROR((B75-C75)/D75),0,(B75*Constantes!$B$26-C75*Constantes!$B$30)/D75)</f>
+      <c r="B72" s="102">
+        <f>('Tablas Calculadas '!C15*Constantes!$D$10*Constantes!$B$10+'Tablas Calculadas '!$D$15*Constantes!D11*Constantes!$B$11+'Tablas Calculadas '!E15*Constantes!$D$12*Constantes!$B$12)*(Constantes!$B$35*(1+Constantes!$E$3)*Constantes!B26)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="17">
-        <f>IF(ISERROR((B76-C76)/D76),0,(B76*Constantes!$B$26-C76*Constantes!$B$30)/D76)</f>
+      <c r="C72" s="6"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="103">
+        <f>('Tablas Calculadas '!C16*Constantes!$D$10*Constantes!$B$10+'Tablas Calculadas '!$D$15*Constantes!D12*Constantes!$B$11+'Tablas Calculadas '!E16*Constantes!$D$12*Constantes!$B$12)*(Constantes!$B$35*(1+Constantes!$E$3)*Constantes!B27)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="17">
-        <f>IF(ISERROR((B77-C77)/D77),0,(B77*Constantes!$B$26-C77*Constantes!$B$30)/D77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="17">
-        <f>IF(ISERROR((B78-C78)/D78),0,(B78*Constantes!$B$26-C78*Constantes!$B$30)/D78)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="17">
-        <f>IF(ISERROR((B79-C79)/D79),0,(B79*Constantes!$B$26-C79*Constantes!$B$30)/D79)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="17">
-        <f>IF(ISERROR((B80-C80)/D80),0,(B80*Constantes!$B$26-C80*Constantes!$B$30)/D80)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="12"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="17">
-        <f>IF(ISERROR((B81-C81)/D81),0,(B81*Constantes!$B$26-C81*Constantes!$B$30)/D81)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="17">
-        <f>IF(ISERROR((B82-C82)/D82),0,(B82*Constantes!$B$26-C82*Constantes!$B$30)/D82)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="12"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="17">
-        <f>IF(ISERROR((B83-C83)/D83),0,(B83*Constantes!$B$26-C83*Constantes!$B$30)/D83)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="17">
-        <f>IF(ISERROR((B84-C84)/D84),0,(B84*Constantes!$B$26-C84*Constantes!$B$30)/D84)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="12"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="17">
-        <f>IF(ISERROR((B85-C85)/D85),0,(B85*Constantes!$B$26-C85*Constantes!$B$30)/D85)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="17">
-        <f>IF(ISERROR((B86-C86)/D86),0,(B86*Constantes!$B$26-C86*Constantes!$B$30)/D86)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="17">
-        <f>IF(ISERROR((B87-C87)/D87),0,(B87*Constantes!$B$26-C87*Constantes!$B$30)/D87)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="17">
-        <f>IF(ISERROR((B88-C88)/D88),0,(B88*Constantes!$B$26-C88*Constantes!$B$30)/D88)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="12"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="17">
-        <f>IF(ISERROR((B89-C89)/D89),0,(B89*Constantes!$B$26-C89*Constantes!$B$30)/D89)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="12"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="17">
-        <f>IF(ISERROR((B90-C90)/D90),0,(B90*Constantes!$B$26-C90*Constantes!$B$30)/D90)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="12"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="17">
-        <f>IF(ISERROR((B91-C91)/D91),0,(B91*Constantes!$B$26-C91*Constantes!$B$30)/D91)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="17">
-        <f>IF(ISERROR((B92-C92)/D92),0,(B92*Constantes!$B$26-C92*Constantes!$B$30)/D92)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="12"/>
-      <c r="C93" s="12"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="17">
-        <f>IF(ISERROR((B93-C93)/D93),0,(B93*Constantes!$B$26-C93*Constantes!$B$30)/D93)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="7"/>
-      <c r="B94" s="12"/>
-      <c r="C94" s="12"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="17">
-        <f>IF(ISERROR((B94-C94)/D94),0,(B94*Constantes!$B$26-C94*Constantes!$B$30)/D94)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="12"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="17">
-        <f>IF(ISERROR((B95-C95)/D95),0,(B95*Constantes!$B$26-C95*Constantes!$B$30)/D95)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="12"/>
-      <c r="C96" s="12"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="17">
-        <f>IF(ISERROR((B96-C96)/D96),0,(B96*Constantes!$B$26-C96*Constantes!$B$30)/D96)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="12"/>
-      <c r="C97" s="12"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="17">
-        <f>IF(ISERROR((B97-C97)/D97),0,(B97*Constantes!$B$26-C97*Constantes!$B$30)/D97)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="14"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="18"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="20">
-        <f>IF(ISERROR((B98-C98)/D98),0,(B98*Constantes!$B$26-C98*Constantes!$B$30)/D98)</f>
-        <v>0</v>
-      </c>
+      <c r="C73" s="6"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" s="103">
+        <f>('Tablas Calculadas '!C17*Constantes!$D$10*Constantes!$B$10+'Tablas Calculadas '!$D$15*Constantes!D13*Constantes!$B$11+'Tablas Calculadas '!E17*Constantes!$D$12*Constantes!$B$12)*(Constantes!$B$35*(1+Constantes!$E$3)*Constantes!B28)</f>
+        <v>244224</v>
+      </c>
+      <c r="C74" s="6"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75" s="103">
+        <f>('Tablas Calculadas '!C18*Constantes!$D$10*Constantes!$B$10+'Tablas Calculadas '!$D$15*Constantes!D14*Constantes!$B$11+'Tablas Calculadas '!E18*Constantes!$D$12*Constantes!$B$12)*(Constantes!$B$35*(1+Constantes!$E$3)*Constantes!B29)</f>
+        <v>258048</v>
+      </c>
+      <c r="C75" s="6"/>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B76" s="104">
+        <f>('Tablas Calculadas '!C19*Constantes!$D$10*Constantes!$B$10+'Tablas Calculadas '!$D$15*Constantes!D15*Constantes!$B$11+'Tablas Calculadas '!E19*Constantes!$D$12*Constantes!$B$12)*(Constantes!$B$35*(1+Constantes!$E$3)*Constantes!B30)</f>
+        <v>884736</v>
+      </c>
+      <c r="C76" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:E68"/>
+  <mergeCells count="21">
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="F6:F8"/>
     <mergeCell ref="J14:J20"/>
@@ -4751,12 +4338,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="A4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4766,10 +4347,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C9FA06-C80F-4B9F-ADFC-C5C56255607A}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4781,67 +4362,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="148.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="A1" s="171" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="173"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="99" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="101"/>
-      <c r="E3" s="145">
+      <c r="C3" s="160" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="162"/>
+      <c r="E3" s="105">
         <v>1</v>
       </c>
-      <c r="F3" s="165" t="s">
-        <v>132</v>
+      <c r="F3" s="108" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="99" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="101"/>
+      <c r="A4" s="160" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="162"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="115">
+        <v>70</v>
+      </c>
+      <c r="B5" s="84">
         <v>50000</v>
       </c>
-      <c r="C5" s="166" t="s">
-        <v>134</v>
+      <c r="C5" s="174" t="s">
+        <v>132</v>
       </c>
       <c r="D5" s="39"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B6" s="12">
         <v>100000</v>
       </c>
-      <c r="C6" s="167"/>
+      <c r="C6" s="175"/>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" s="12">
         <v>150000</v>
       </c>
-      <c r="C7" s="168"/>
+      <c r="C7" s="176"/>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4851,38 +4432,38 @@
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="114" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="119" t="s">
-        <v>97</v>
-      </c>
-      <c r="C9" s="119" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="119" t="s">
+      <c r="A9" s="83" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="85" t="s">
         <v>95</v>
       </c>
+      <c r="C9" s="85" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="85" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="93">
+      <c r="A10" s="86" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="70">
         <v>12</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>
       </c>
-      <c r="D10" s="122">
+      <c r="D10" s="88">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" s="94">
+      <c r="A11" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="71">
         <v>24</v>
       </c>
       <c r="C11" s="1">
@@ -4893,8 +4474,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="121" t="s">
-        <v>81</v>
+      <c r="A12" s="87" t="s">
+        <v>79</v>
       </c>
       <c r="B12" s="14">
         <v>32</v>
@@ -4905,8 +4486,8 @@
       <c r="D12" s="20">
         <v>9</v>
       </c>
-      <c r="E12" s="165" t="s">
-        <v>137</v>
+      <c r="E12" s="108" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -4933,43 +4514,43 @@
       <c r="D16" s="38"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="160" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="161"/>
+      <c r="C17" s="161"/>
+      <c r="D17" s="162"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="180" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="180"/>
+      <c r="C18" s="85" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="181" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="100"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="101"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="123" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="123"/>
-      <c r="C18" s="119" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="119" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="B19" s="182"/>
+      <c r="C19" s="89">
+        <v>657</v>
+      </c>
+      <c r="D19" s="88">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="183" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="124"/>
-      <c r="C19" s="129">
-        <v>657</v>
-      </c>
-      <c r="D19" s="122">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="125" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="126"/>
-      <c r="C20" s="130">
+      <c r="B20" s="184"/>
+      <c r="C20" s="90">
         <v>200</v>
       </c>
       <c r="D20" s="17">
@@ -4977,11 +4558,11 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="125" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="126"/>
-      <c r="C21" s="130">
+      <c r="A21" s="183" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="184"/>
+      <c r="C21" s="90">
         <v>150</v>
       </c>
       <c r="D21" s="17">
@@ -4989,11 +4570,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="127" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="128"/>
-      <c r="C22" s="131">
+      <c r="A22" s="185" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="186"/>
+      <c r="C22" s="91">
         <f>SUM(C19:C21)</f>
         <v>1007</v>
       </c>
@@ -5006,32 +4587,32 @@
       <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="101"/>
+      <c r="A24" s="160" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="162"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="119" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="119" t="s">
-        <v>56</v>
+      <c r="A25" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="85" t="s">
+        <v>55</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="132">
+      <c r="A26" s="92">
         <v>0</v>
       </c>
-      <c r="B26" s="133">
+      <c r="B26" s="93">
         <v>40</v>
       </c>
-      <c r="C26" s="162" t="s">
-        <v>139</v>
+      <c r="C26" s="177" t="s">
+        <v>137</v>
       </c>
       <c r="D26" s="6"/>
     </row>
@@ -5042,7 +4623,7 @@
       <c r="B27" s="36">
         <v>46</v>
       </c>
-      <c r="C27" s="163"/>
+      <c r="C27" s="178"/>
       <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -5052,7 +4633,7 @@
       <c r="B28" s="36">
         <v>53</v>
       </c>
-      <c r="C28" s="163"/>
+      <c r="C28" s="178"/>
       <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -5062,17 +4643,17 @@
       <c r="B29" s="36">
         <v>56</v>
       </c>
-      <c r="C29" s="163"/>
+      <c r="C29" s="178"/>
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>4</v>
       </c>
-      <c r="B30" s="134">
+      <c r="B30" s="94">
         <v>64</v>
       </c>
-      <c r="C30" s="164"/>
+      <c r="C30" s="179"/>
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,18 +4675,18 @@
       <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="99" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="101"/>
+      <c r="A34" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="162"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="135" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="136">
+      <c r="A35" s="95" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="96">
         <v>8</v>
       </c>
       <c r="C35" s="6"/>
@@ -5113,43 +4694,43 @@
     </row>
     <row r="36" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B36" s="137">
+        <v>96</v>
+      </c>
+      <c r="B36" s="97">
         <v>16</v>
       </c>
-      <c r="C36" s="165" t="s">
-        <v>141</v>
+      <c r="C36" s="108" t="s">
+        <v>139</v>
       </c>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="138">
+        <v>42</v>
+      </c>
+      <c r="B37" s="98">
         <v>8</v>
       </c>
-      <c r="C37" s="169" t="s">
-        <v>143</v>
+      <c r="C37" s="132" t="s">
+        <v>141</v>
       </c>
       <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="138">
+        <v>43</v>
+      </c>
+      <c r="B38" s="98">
         <v>22</v>
       </c>
-      <c r="C38" s="170"/>
+      <c r="C38" s="134"/>
       <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="138">
+        <v>45</v>
+      </c>
+      <c r="B39" s="98">
         <v>4</v>
       </c>
       <c r="C39" s="6"/>
@@ -5157,7 +4738,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="36">
         <f>(B35*B26*B37*B38*B39)*(1+(B48+B49+B50))</f>
@@ -5168,7 +4749,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="36">
         <f>(B35*B27*B37*B38*B39)*(1+(B48+B49+B50))</f>
@@ -5179,7 +4760,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B42" s="36">
         <f>(B35*B28*B37*B38*B39)*(1+(B48+B49+B50))</f>
@@ -5190,7 +4771,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="36">
         <f>(B35*B29*B37*B38*B39)*(1+(B48+B49+B50))</f>
@@ -5201,7 +4782,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="36">
         <f>(B35*B30*B37*B38*B39)*(1+(B48+B49+B50))</f>
@@ -5212,9 +4793,9 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="137">
+        <v>73</v>
+      </c>
+      <c r="B45" s="97">
         <v>150</v>
       </c>
       <c r="C45" s="6"/>
@@ -5222,9 +4803,9 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="137">
+        <v>74</v>
+      </c>
+      <c r="B46" s="97">
         <v>500</v>
       </c>
       <c r="C46" s="6"/>
@@ -5232,9 +4813,9 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B47" s="137">
+        <v>59</v>
+      </c>
+      <c r="B47" s="97">
         <v>250</v>
       </c>
       <c r="C47" s="6"/>
@@ -5242,113 +4823,406 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="139">
+        <v>75</v>
+      </c>
+      <c r="B48" s="99">
         <v>0.03</v>
       </c>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B49" s="139">
+        <v>76</v>
+      </c>
+      <c r="B49" s="99">
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="140" t="s">
-        <v>79</v>
-      </c>
-      <c r="B50" s="141">
+    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="101">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="99" t="s">
-        <v>105</v>
-      </c>
-      <c r="B53" s="101"/>
-      <c r="C53" s="171" t="s">
-        <v>145</v>
-      </c>
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="132" t="s">
-        <v>6</v>
-      </c>
-      <c r="B54" s="142">
-        <f>(Hoja2!C15*$D$10*$B$10+Hoja2!$D$15*D11*$B$11+Hoja2!E15*$D$12*$B$12)*($B$35*(1+Constantes!$E$3)*B26)</f>
+    <row r="53" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="127" t="s">
+        <v>40</v>
+      </c>
+      <c r="B53" s="128"/>
+      <c r="C53" s="127" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="129"/>
+      <c r="E53" s="128"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="12">
+        <v>425</v>
+      </c>
+      <c r="C55" s="12">
+        <v>180</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5</v>
+      </c>
+      <c r="E55" s="17">
+        <f>IF(ISERROR((B55-C55)/D55),0,(B55*Constantes!$B$26-C55*Constantes!$B$30)/D55)</f>
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="12">
+        <v>125</v>
+      </c>
+      <c r="C56" s="12">
+        <v>40</v>
+      </c>
+      <c r="D56" s="1">
+        <v>10</v>
+      </c>
+      <c r="E56" s="17">
+        <f>IF(ISERROR((B56-C56)/D56),0,(B56*Constantes!$B$26-C56*Constantes!$B$30)/D56)</f>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="12">
+        <v>66</v>
+      </c>
+      <c r="C57" s="12">
+        <v>15</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="E57" s="17">
+        <f>IF(ISERROR((B57-C57)/D57),0,(B57*Constantes!$B$26-C57*Constantes!$B$30)/D57)</f>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" s="12">
+        <v>279</v>
+      </c>
+      <c r="C58" s="12">
+        <v>110</v>
+      </c>
+      <c r="D58" s="1">
+        <v>5</v>
+      </c>
+      <c r="E58" s="17">
+        <f>IF(ISERROR((B58-C58)/D58),0,(B58*Constantes!$B$26-C58*Constantes!$B$30)/D58)</f>
+        <v>824</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="12">
+        <v>95</v>
+      </c>
+      <c r="C59" s="12">
+        <v>15</v>
+      </c>
+      <c r="D59" s="1">
+        <v>10</v>
+      </c>
+      <c r="E59" s="17">
+        <f>IF(ISERROR((B59-C59)/D59),0,(B59*Constantes!$B$26-C59*Constantes!B28)/D59)</f>
+        <v>300.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="17">
+        <f>IF(ISERROR((B60-C60)/D60),0,(B60*Constantes!$B$26-C60*Constantes!$B$30)/D60)</f>
         <v>0</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="143">
-        <f>(Hoja2!C16*$D$10*$B$10+Hoja2!$D$15*D12*$B$11+Hoja2!E16*$D$12*$B$12)*($B$35*(1+Constantes!$E$3)*B27)</f>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="17">
+        <f>IF(ISERROR((B61-C61)/D61),0,(B61*Constantes!$B$26-C61*Constantes!$B$30)/D61)</f>
         <v>0</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B56" s="143">
-        <f>(Hoja2!C17*$D$10*$B$10+Hoja2!$D$15*D13*$B$11+Hoja2!E17*$D$12*$B$12)*($B$35*(1+Constantes!$E$3)*B28)</f>
-        <v>244224</v>
-      </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57" s="143">
-        <f>(Hoja2!C18*$D$10*$B$10+Hoja2!$D$15*D14*$B$11+Hoja2!E18*$D$12*$B$12)*($B$35*(1+Constantes!$E$3)*B29)</f>
-        <v>258048</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-    </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="144">
-        <f>(Hoja2!C19*$D$10*$B$10+Hoja2!$D$15*D15*$B$11+Hoja2!E19*$D$12*$B$12)*($B$35*(1+Constantes!$E$3)*B30)</f>
-        <v>884736</v>
-      </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="17">
+        <f>IF(ISERROR((B62-C62)/D62),0,(B62*Constantes!$B$26-C62*Constantes!$B$30)/D62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="17">
+        <f>IF(ISERROR((B63-C63)/D63),0,(B63*Constantes!$B$26-C63*Constantes!$B$30)/D63)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="17">
+        <f>IF(ISERROR((B64-C64)/D64),0,(B64*Constantes!$B$26-C64*Constantes!$B$30)/D64)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="17">
+        <f>IF(ISERROR((B65-C65)/D65),0,(B65*Constantes!$B$26-C65*Constantes!$B$30)/D65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="17">
+        <f>IF(ISERROR((B66-C66)/D66),0,(B66*Constantes!$B$26-C66*Constantes!$B$30)/D66)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="17">
+        <f>IF(ISERROR((B67-C67)/D67),0,(B67*Constantes!$B$26-C67*Constantes!$B$30)/D67)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="17">
+        <f>IF(ISERROR((B68-C68)/D68),0,(B68*Constantes!$B$26-C68*Constantes!$B$30)/D68)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="17">
+        <f>IF(ISERROR((B69-C69)/D69),0,(B69*Constantes!$B$26-C69*Constantes!$B$30)/D69)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="17">
+        <f>IF(ISERROR((B70-C70)/D70),0,(B70*Constantes!$B$26-C70*Constantes!$B$30)/D70)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="17">
+        <f>IF(ISERROR((B71-C71)/D71),0,(B71*Constantes!$B$26-C71*Constantes!$B$30)/D71)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="17">
+        <f>IF(ISERROR((B72-C72)/D72),0,(B72*Constantes!$B$26-C72*Constantes!$B$30)/D72)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="17">
+        <f>IF(ISERROR((B73-C73)/D73),0,(B73*Constantes!$B$26-C73*Constantes!$B$30)/D73)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="17">
+        <f>IF(ISERROR((B74-C74)/D74),0,(B74*Constantes!$B$26-C74*Constantes!$B$30)/D74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="17">
+        <f>IF(ISERROR((B75-C75)/D75),0,(B75*Constantes!$B$26-C75*Constantes!$B$30)/D75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="17">
+        <f>IF(ISERROR((B76-C76)/D76),0,(B76*Constantes!$B$26-C76*Constantes!$B$30)/D76)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="17">
+        <f>IF(ISERROR((B77-C77)/D77),0,(B77*Constantes!$B$26-C77*Constantes!$B$30)/D77)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="17">
+        <f>IF(ISERROR((B78-C78)/D78),0,(B78*Constantes!$B$26-C78*Constantes!$B$30)/D78)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="7"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="17">
+        <f>IF(ISERROR((B79-C79)/D79),0,(B79*Constantes!$B$26-C79*Constantes!$B$30)/D79)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="17">
+        <f>IF(ISERROR((B80-C80)/D80),0,(B80*Constantes!$B$26-C80*Constantes!$B$30)/D80)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="17">
+        <f>IF(ISERROR((B81-C81)/D81),0,(B81*Constantes!$B$26-C81*Constantes!$B$30)/D81)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="17">
+        <f>IF(ISERROR((B82-C82)/D82),0,(B82*Constantes!$B$26-C82*Constantes!$B$30)/D82)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="14"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="20">
+        <f>IF(ISERROR((B83-C83)/D83),0,(B83*Constantes!$B$26-C83*Constantes!$B$30)/D83)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A17:D17"/>
@@ -5364,6 +5238,7 @@
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C53:E53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5390,188 +5265,193 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="117" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67"/>
+      <c r="A1" s="171" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="172"/>
+      <c r="C1" s="172"/>
+      <c r="D1" s="172"/>
+      <c r="E1" s="172"/>
+      <c r="F1" s="172"/>
+      <c r="G1" s="172"/>
+      <c r="H1" s="172"/>
+      <c r="I1" s="173"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="160" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="161"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="162"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="110" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="100"/>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="101"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="172" t="s">
+      <c r="B4" s="190" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="191"/>
+      <c r="D4" s="191"/>
+      <c r="E4" s="191"/>
+      <c r="F4" s="191"/>
+      <c r="G4" s="192"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="110" t="s">
         <v>109</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B5" s="188" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="172" t="s">
+      <c r="C5" s="188"/>
+      <c r="D5" s="188"/>
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
+      <c r="G5" s="189"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="110" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="55"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="172" t="s">
-        <v>113</v>
-      </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="188" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="188"/>
+      <c r="D6" s="188"/>
+      <c r="E6" s="188"/>
+      <c r="F6" s="188"/>
+      <c r="G6" s="189"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="110" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="188" t="s">
         <v>129</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="172" t="s">
+      <c r="C7" s="188"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="189"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="110" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B8" s="188" t="s">
         <v>131</v>
       </c>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="172" t="s">
+      <c r="C8" s="188"/>
+      <c r="D8" s="188"/>
+      <c r="E8" s="188"/>
+      <c r="F8" s="188"/>
+      <c r="G8" s="189"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="110" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B9" s="188" t="s">
         <v>133</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="55"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="172" t="s">
+      <c r="C9" s="188"/>
+      <c r="D9" s="188"/>
+      <c r="E9" s="188"/>
+      <c r="F9" s="188"/>
+      <c r="G9" s="189"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="110" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="172" t="s">
+      <c r="B10" s="187" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="C10" s="188"/>
+      <c r="D10" s="188"/>
+      <c r="E10" s="188"/>
+      <c r="F10" s="188"/>
+      <c r="G10" s="189"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="110" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="188" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="55"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="172" t="s">
+      <c r="C11" s="188"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="188"/>
+      <c r="F11" s="188"/>
+      <c r="G11" s="189"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="110" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B12" s="188" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="172" t="s">
+      <c r="C12" s="188"/>
+      <c r="D12" s="188"/>
+      <c r="E12" s="188"/>
+      <c r="F12" s="188"/>
+      <c r="G12" s="189"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="54" t="s">
+      <c r="B13" s="187" t="s">
         <v>142</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="172" t="s">
+      <c r="C13" s="188"/>
+      <c r="D13" s="188"/>
+      <c r="E13" s="188"/>
+      <c r="F13" s="188"/>
+      <c r="G13" s="189"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="110" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B14" s="187" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
-      <c r="G13" s="55"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="172" t="s">
+      <c r="C14" s="188"/>
+      <c r="D14" s="188"/>
+      <c r="E14" s="188"/>
+      <c r="F14" s="188"/>
+      <c r="G14" s="189"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="110" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="55"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="172" t="s">
+      <c r="B15" s="193" t="s">
         <v>147</v>
       </c>
-      <c r="B15" s="68" t="s">
-        <v>149</v>
-      </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
+      <c r="C15" s="193"/>
+      <c r="D15" s="193"/>
+      <c r="E15" s="193"/>
+      <c r="F15" s="193"/>
+      <c r="G15" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B5:G5"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="B11:G11"/>
     <mergeCell ref="A3:G3"/>
@@ -5581,11 +5461,6 @@
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>